<commit_message>
fix error in tb limit formula
</commit_message>
<xml_diff>
--- a/testsheets/666_Keysight_DSOX3034A.xlsx
+++ b/testsheets/666_Keysight_DSOX3034A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Python\oscilloscope\testsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E285BBD7-B79C-449E-A18F-9BFD312E3B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{41BC0363-D29C-4916-A505-2A820B85EFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="72">
   <si>
     <t>EMU Filename:</t>
   </si>
@@ -106,9 +106,6 @@
     <t>ISSUE:</t>
   </si>
   <si>
-    <t>A.00.02</t>
-  </si>
-  <si>
     <t>DC Vertical Measurement Accuracy</t>
   </si>
   <si>
@@ -133,34 +130,10 @@
     <t>Pass/Fail</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>Coupling</t>
-  </si>
-  <si>
-    <t>Scale</t>
-  </si>
-  <si>
-    <t>Voltage</t>
-  </si>
-  <si>
-    <t>Offset</t>
-  </si>
-  <si>
     <t>Channel 1</t>
   </si>
   <si>
     <t>V</t>
-  </si>
-  <si>
-    <t>DCV</t>
-  </si>
-  <si>
-    <t>DC</t>
   </si>
   <si>
     <t>mV</t>
@@ -178,39 +151,7 @@
     <t>Dual Cursor Accuracy</t>
   </si>
   <si>
-    <t>CURS</t>
-  </si>
-  <si>
     <t>Analog Bandwidth</t>
-  </si>
-  <si>
-    <t>Test Conditions</t>
-  </si>
-  <si>
-    <t>Rise Time
-(Measured)</t>
-  </si>
-  <si>
-    <t>Lower Limit</t>
-  </si>
-  <si>
-    <t>Bandwidth
-(Calculated)</t>
-  </si>
-  <si>
-    <t>Channel 1 (350 MHz)</t>
-  </si>
-  <si>
-    <t>MHz</t>
-  </si>
-  <si>
-    <t>Channel 2 (350 MHz)</t>
-  </si>
-  <si>
-    <t>Channel 3 (350 MHz)</t>
-  </si>
-  <si>
-    <t>Channel 4 (350 MHz)</t>
   </si>
   <si>
     <t>Time Base Accuracy</t>
@@ -223,9 +164,6 @@
   </si>
   <si>
     <t>Limit</t>
-  </si>
-  <si>
-    <t>TIME</t>
   </si>
   <si>
     <t>Trigger Sensitivity</t>
@@ -253,6 +191,71 @@
   </si>
   <si>
     <t>END OF REPORT</t>
+  </si>
+  <si>
+    <t>Test Conditions</t>
+  </si>
+  <si>
+    <t>A.00.02</t>
+  </si>
+  <si>
+    <t>Channel 1 (350 MHz)</t>
+  </si>
+  <si>
+    <t>Channel 2 (350 MHz)</t>
+  </si>
+  <si>
+    <t>Channel 3 (350 MHz)</t>
+  </si>
+  <si>
+    <t>Channel 4 (350 MHz)</t>
+  </si>
+  <si>
+    <t>Rise Time
+(Measured)</t>
+  </si>
+  <si>
+    <t>Lower Limit</t>
+  </si>
+  <si>
+    <t>Bandwidth
+(Calculated)</t>
+  </si>
+  <si>
+    <t>MHz</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Coupling</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>DCV</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>CURS</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>Timebase (ns)</t>
   </si>
 </sst>
 </file>
@@ -2464,7 +2467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -2554,58 +2557,58 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="K14" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="L14" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="M14" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="N14" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="O14" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="P14" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -2629,20 +2632,20 @@
         <v>36.200000000000003</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G16" s="10" t="str">
         <f t="shared" ref="G16:G26" si="0">IF(ISBLANK(D16),"Not Done",IF(AND(D16&lt;=E16,D16&gt;=C16),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
       <c r="K16" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L16">
         <v>1</v>
       </c>
       <c r="M16" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N16">
         <v>5</v>
@@ -2669,20 +2672,20 @@
         <v>14.48</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G17" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K17" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L17">
         <v>1</v>
       </c>
       <c r="M17" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -2709,20 +2712,20 @@
         <v>7.24</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G18" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K18" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L18">
         <v>1</v>
       </c>
       <c r="M18" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -2749,20 +2752,20 @@
         <v>3.62</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G19" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K19" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L19">
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N19">
         <v>0.5</v>
@@ -2789,20 +2792,20 @@
         <v>1.448</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G20" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K20" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L20">
         <v>1</v>
       </c>
       <c r="M20" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N20">
         <v>0.2</v>
@@ -2829,20 +2832,20 @@
         <v>724</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G21" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K21" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L21">
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N21">
         <v>0.1</v>
@@ -2851,7 +2854,7 @@
         <v>0.7</v>
       </c>
       <c r="P21">
-        <v>0.35</v>
+        <v>0.35000000000000003</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -2869,20 +2872,20 @@
         <v>362</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G22" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K22" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L22">
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N22">
         <v>0.05</v>
@@ -2891,7 +2894,7 @@
         <v>0.35</v>
       </c>
       <c r="P22">
-        <v>0.17499999999999999</v>
+        <v>0.17500000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -2909,20 +2912,20 @@
         <v>144.80000000000001</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G23" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K23" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L23">
         <v>1</v>
       </c>
       <c r="M23" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N23">
         <v>0.02</v>
@@ -2949,20 +2952,20 @@
         <v>72.400000000000006</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G24" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K24" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L24">
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N24">
         <v>0.01</v>
@@ -2989,20 +2992,20 @@
         <v>36.6</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G25" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K25" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L25">
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N25">
         <v>5.0000000000000001E-3</v>
@@ -3029,20 +3032,20 @@
         <v>15.28</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G26" s="10" t="str">
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
       <c r="K26" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L26">
         <v>1</v>
       </c>
       <c r="M26" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N26">
         <v>2E-3</v>
@@ -3056,7 +3059,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -3080,20 +3083,20 @@
         <v>36.200000000000003</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G28" s="10" t="str">
         <f t="shared" ref="G28:G38" si="1">IF(ISBLANK(D28),"Not Done",IF(AND(D28&lt;=E28,D28&gt;=C28),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
       <c r="K28" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L28">
         <v>2</v>
       </c>
       <c r="M28" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N28">
         <v>5</v>
@@ -3120,20 +3123,20 @@
         <v>14.48</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G29" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K29" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L29">
         <v>2</v>
       </c>
       <c r="M29" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N29">
         <v>2</v>
@@ -3160,20 +3163,20 @@
         <v>7.24</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G30" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K30" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L30">
         <v>2</v>
       </c>
       <c r="M30" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N30">
         <v>1</v>
@@ -3200,20 +3203,20 @@
         <v>3.62</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G31" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K31" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L31">
         <v>2</v>
       </c>
       <c r="M31" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N31">
         <v>0.5</v>
@@ -3240,20 +3243,20 @@
         <v>1.448</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G32" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K32" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L32">
         <v>2</v>
       </c>
       <c r="M32" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N32">
         <v>0.2</v>
@@ -3280,20 +3283,20 @@
         <v>724</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G33" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K33" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L33">
         <v>2</v>
       </c>
       <c r="M33" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N33">
         <v>0.1</v>
@@ -3302,7 +3305,7 @@
         <v>0.7</v>
       </c>
       <c r="P33">
-        <v>0.35</v>
+        <v>0.35000000000000003</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -3320,20 +3323,20 @@
         <v>362</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G34" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K34" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L34">
         <v>2</v>
       </c>
       <c r="M34" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N34">
         <v>0.05</v>
@@ -3342,7 +3345,7 @@
         <v>0.35</v>
       </c>
       <c r="P34">
-        <v>0.17499999999999999</v>
+        <v>0.17500000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -3360,20 +3363,20 @@
         <v>144.80000000000001</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G35" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K35" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L35">
         <v>2</v>
       </c>
       <c r="M35" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N35">
         <v>0.02</v>
@@ -3400,20 +3403,20 @@
         <v>72.400000000000006</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G36" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K36" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L36">
         <v>2</v>
       </c>
       <c r="M36" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N36">
         <v>0.01</v>
@@ -3440,20 +3443,20 @@
         <v>36.6</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G37" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K37" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L37">
         <v>2</v>
       </c>
       <c r="M37" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N37">
         <v>5.0000000000000001E-3</v>
@@ -3480,20 +3483,20 @@
         <v>15.28</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G38" s="10" t="str">
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
       <c r="K38" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L38">
         <v>2</v>
       </c>
       <c r="M38" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N38">
         <v>2E-3</v>
@@ -3507,7 +3510,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -3531,20 +3534,20 @@
         <v>36.200000000000003</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G40" s="10" t="str">
         <f t="shared" ref="G40:G50" si="2">IF(ISBLANK(D40),"Not Done",IF(AND(D40&lt;=E40,D40&gt;=C40),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
       <c r="K40" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L40">
         <v>3</v>
       </c>
       <c r="M40" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N40">
         <v>5</v>
@@ -3571,20 +3574,20 @@
         <v>14.48</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G41" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K41" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L41">
         <v>3</v>
       </c>
       <c r="M41" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N41">
         <v>2</v>
@@ -3611,20 +3614,20 @@
         <v>7.24</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G42" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K42" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L42">
         <v>3</v>
       </c>
       <c r="M42" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N42">
         <v>1</v>
@@ -3651,20 +3654,20 @@
         <v>3.62</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G43" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K43" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L43">
         <v>3</v>
       </c>
       <c r="M43" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N43">
         <v>0.5</v>
@@ -3691,20 +3694,20 @@
         <v>1.448</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G44" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K44" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L44">
         <v>3</v>
       </c>
       <c r="M44" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N44">
         <v>0.2</v>
@@ -3731,20 +3734,20 @@
         <v>724</v>
       </c>
       <c r="F45" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G45" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K45" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L45">
         <v>3</v>
       </c>
       <c r="M45" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N45">
         <v>0.1</v>
@@ -3753,7 +3756,7 @@
         <v>0.7</v>
       </c>
       <c r="P45">
-        <v>0.35</v>
+        <v>0.35000000000000003</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3771,20 +3774,20 @@
         <v>362</v>
       </c>
       <c r="F46" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G46" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K46" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L46">
         <v>3</v>
       </c>
       <c r="M46" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N46">
         <v>0.05</v>
@@ -3793,7 +3796,7 @@
         <v>0.35</v>
       </c>
       <c r="P46">
-        <v>0.17499999999999999</v>
+        <v>0.17500000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3811,20 +3814,20 @@
         <v>144.80000000000001</v>
       </c>
       <c r="F47" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G47" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K47" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L47">
         <v>3</v>
       </c>
       <c r="M47" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N47">
         <v>0.02</v>
@@ -3851,20 +3854,20 @@
         <v>72.400000000000006</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G48" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K48" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L48">
         <v>3</v>
       </c>
       <c r="M48" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N48">
         <v>0.01</v>
@@ -3891,20 +3894,20 @@
         <v>36.6</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G49" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K49" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L49">
         <v>3</v>
       </c>
       <c r="M49" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N49">
         <v>5.0000000000000001E-3</v>
@@ -3931,20 +3934,20 @@
         <v>15.28</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G50" s="10" t="str">
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
       <c r="K50" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L50">
         <v>3</v>
       </c>
       <c r="M50" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N50">
         <v>2E-3</v>
@@ -3958,7 +3961,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -3982,20 +3985,20 @@
         <v>36.200000000000003</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G52" s="10" t="str">
         <f t="shared" ref="G52:G62" si="3">IF(ISBLANK(D52),"Not Done",IF(AND(D52&lt;=E52,D52&gt;=C52),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
       <c r="K52" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L52">
         <v>4</v>
       </c>
       <c r="M52" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N52">
         <v>5</v>
@@ -4022,20 +4025,20 @@
         <v>14.28</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G53" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K53" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L53">
         <v>4</v>
       </c>
       <c r="M53" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N53">
         <v>2</v>
@@ -4062,20 +4065,20 @@
         <v>7.24</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G54" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K54" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L54">
         <v>4</v>
       </c>
       <c r="M54" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N54">
         <v>1</v>
@@ -4102,20 +4105,20 @@
         <v>3.62</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G55" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K55" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L55">
         <v>4</v>
       </c>
       <c r="M55" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N55">
         <v>0.5</v>
@@ -4142,20 +4145,20 @@
         <v>1.448</v>
       </c>
       <c r="F56" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G56" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K56" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L56">
         <v>4</v>
       </c>
       <c r="M56" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N56">
         <v>0.2</v>
@@ -4182,20 +4185,20 @@
         <v>724</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G57" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K57" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L57">
         <v>4</v>
       </c>
       <c r="M57" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N57">
         <v>0.1</v>
@@ -4204,7 +4207,7 @@
         <v>0.7</v>
       </c>
       <c r="P57">
-        <v>0.35</v>
+        <v>0.35000000000000003</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -4222,20 +4225,20 @@
         <v>362</v>
       </c>
       <c r="F58" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G58" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K58" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L58">
         <v>4</v>
       </c>
       <c r="M58" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N58">
         <v>0.05</v>
@@ -4244,7 +4247,7 @@
         <v>0.35</v>
       </c>
       <c r="P58">
-        <v>0.17499999999999999</v>
+        <v>0.17500000000000002</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -4262,20 +4265,20 @@
         <v>144.80000000000001</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G59" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K59" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L59">
         <v>4</v>
       </c>
       <c r="M59" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N59">
         <v>0.02</v>
@@ -4302,20 +4305,20 @@
         <v>72.400000000000006</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G60" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K60" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L60">
         <v>4</v>
       </c>
       <c r="M60" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N60">
         <v>0.01</v>
@@ -4342,20 +4345,20 @@
         <v>36.6</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G61" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K61" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L61">
         <v>4</v>
       </c>
       <c r="M61" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N61">
         <v>5.0000000000000001E-3</v>
@@ -4382,20 +4385,20 @@
         <v>15.28</v>
       </c>
       <c r="F62" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G62" s="10" t="str">
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
       <c r="K62" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="L62">
         <v>4</v>
       </c>
       <c r="M62" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N62">
         <v>2E-3</v>
@@ -4407,37 +4410,37 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="C65" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="D65" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="E65" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E65" s="5" t="s">
+      <c r="F65" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F65" s="5" t="s">
+      <c r="G65" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="G65" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -4461,20 +4464,20 @@
         <v>36.4</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G67" s="10" t="str">
         <f t="shared" ref="G67:G77" si="4">IF(ISBLANK(D67),"Not Done",IF(AND(D67&lt;=E67,D67&gt;=C67),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
       <c r="K67" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L67">
         <v>1</v>
       </c>
       <c r="M67" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N67">
         <v>5</v>
@@ -4501,20 +4504,20 @@
         <v>14.56</v>
       </c>
       <c r="F68" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G68" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K68" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L68">
         <v>1</v>
       </c>
       <c r="M68" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N68">
         <v>2</v>
@@ -4541,20 +4544,20 @@
         <v>7.28</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G69" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K69" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L69">
         <v>1</v>
       </c>
       <c r="M69" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N69">
         <v>1</v>
@@ -4581,20 +4584,20 @@
         <v>3.64</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G70" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K70" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L70">
         <v>1</v>
       </c>
       <c r="M70" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N70">
         <v>0.5</v>
@@ -4621,20 +4624,20 @@
         <v>1.456</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G71" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K71" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L71">
         <v>1</v>
       </c>
       <c r="M71" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N71">
         <v>0.2</v>
@@ -4661,20 +4664,20 @@
         <v>728</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G72" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K72" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L72">
         <v>1</v>
       </c>
       <c r="M72" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N72">
         <v>0.1</v>
@@ -4683,7 +4686,7 @@
         <v>0.7</v>
       </c>
       <c r="P72">
-        <v>0.35</v>
+        <v>0.35000000000000003</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -4701,20 +4704,20 @@
         <v>364</v>
       </c>
       <c r="F73" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G73" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K73" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L73">
         <v>1</v>
       </c>
       <c r="M73" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N73">
         <v>0.05</v>
@@ -4723,7 +4726,7 @@
         <v>0.35</v>
       </c>
       <c r="P73">
-        <v>0.17499999999999999</v>
+        <v>0.17500000000000002</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
@@ -4741,20 +4744,20 @@
         <v>145.6</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G74" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K74" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L74">
         <v>1</v>
       </c>
       <c r="M74" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N74">
         <v>0.02</v>
@@ -4781,20 +4784,20 @@
         <v>72.8</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G75" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K75" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L75">
         <v>1</v>
       </c>
       <c r="M75" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N75">
         <v>0.01</v>
@@ -4821,20 +4824,20 @@
         <v>36.799999999999997</v>
       </c>
       <c r="F76" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G76" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K76" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L76">
         <v>1</v>
       </c>
       <c r="M76" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N76">
         <v>5.0000000000000001E-3</v>
@@ -4861,20 +4864,20 @@
         <v>15.44</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G77" s="10" t="str">
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
       <c r="K77" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L77">
         <v>1</v>
       </c>
       <c r="M77" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N77">
         <v>2E-3</v>
@@ -4888,7 +4891,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -4912,20 +4915,20 @@
         <v>36.4</v>
       </c>
       <c r="F79" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G79" s="10" t="str">
         <f t="shared" ref="G79:G89" si="5">IF(ISBLANK(D79),"Not Done",IF(AND(D79&lt;=E79,D79&gt;=C79),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
       <c r="K79" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L79">
         <v>2</v>
       </c>
       <c r="M79" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N79">
         <v>5</v>
@@ -4952,20 +4955,20 @@
         <v>14.56</v>
       </c>
       <c r="F80" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G80" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K80" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L80">
         <v>2</v>
       </c>
       <c r="M80" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N80">
         <v>2</v>
@@ -4992,20 +4995,20 @@
         <v>7.28</v>
       </c>
       <c r="F81" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G81" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K81" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L81">
         <v>2</v>
       </c>
       <c r="M81" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N81">
         <v>1</v>
@@ -5032,20 +5035,20 @@
         <v>3.64</v>
       </c>
       <c r="F82" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G82" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K82" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L82">
         <v>2</v>
       </c>
       <c r="M82" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N82">
         <v>0.5</v>
@@ -5072,20 +5075,20 @@
         <v>1.456</v>
       </c>
       <c r="F83" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G83" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K83" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L83">
         <v>2</v>
       </c>
       <c r="M83" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N83">
         <v>0.2</v>
@@ -5112,20 +5115,20 @@
         <v>728</v>
       </c>
       <c r="F84" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G84" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K84" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L84">
         <v>2</v>
       </c>
       <c r="M84" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N84">
         <v>0.1</v>
@@ -5134,7 +5137,7 @@
         <v>0.7</v>
       </c>
       <c r="P84">
-        <v>0.35</v>
+        <v>0.35000000000000003</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -5152,20 +5155,20 @@
         <v>362</v>
       </c>
       <c r="F85" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G85" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K85" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L85">
         <v>2</v>
       </c>
       <c r="M85" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N85">
         <v>0.05</v>
@@ -5174,7 +5177,7 @@
         <v>0.35</v>
       </c>
       <c r="P85">
-        <v>0.17499999999999999</v>
+        <v>0.17500000000000002</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
@@ -5192,20 +5195,20 @@
         <v>145.6</v>
       </c>
       <c r="F86" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G86" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K86" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L86">
         <v>2</v>
       </c>
       <c r="M86" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N86">
         <v>0.02</v>
@@ -5232,20 +5235,20 @@
         <v>72.8</v>
       </c>
       <c r="F87" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G87" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K87" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L87">
         <v>2</v>
       </c>
       <c r="M87" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N87">
         <v>0.01</v>
@@ -5272,20 +5275,20 @@
         <v>36.799999999999997</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G88" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K88" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L88">
         <v>2</v>
       </c>
       <c r="M88" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N88">
         <v>5.0000000000000001E-3</v>
@@ -5312,20 +5315,20 @@
         <v>15.44</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G89" s="10" t="str">
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
       <c r="K89" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L89">
         <v>2</v>
       </c>
       <c r="M89" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N89">
         <v>2E-3</v>
@@ -5339,7 +5342,7 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -5363,20 +5366,20 @@
         <v>36.4</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G91" s="10" t="str">
         <f t="shared" ref="G91:G101" si="6">IF(ISBLANK(D91),"Not Done",IF(AND(D91&lt;=E91,D91&gt;=C91),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
       <c r="K91" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L91">
         <v>3</v>
       </c>
       <c r="M91" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N91">
         <v>5</v>
@@ -5403,20 +5406,20 @@
         <v>14.56</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G92" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K92" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L92">
         <v>3</v>
       </c>
       <c r="M92" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N92">
         <v>2</v>
@@ -5443,20 +5446,20 @@
         <v>7.28</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G93" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K93" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L93">
         <v>3</v>
       </c>
       <c r="M93" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N93">
         <v>1</v>
@@ -5483,20 +5486,20 @@
         <v>3.64</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G94" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K94" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L94">
         <v>3</v>
       </c>
       <c r="M94" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N94">
         <v>0.5</v>
@@ -5523,20 +5526,20 @@
         <v>1.456</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G95" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K95" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L95">
         <v>3</v>
       </c>
       <c r="M95" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N95">
         <v>0.2</v>
@@ -5563,20 +5566,20 @@
         <v>728</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G96" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K96" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L96">
         <v>3</v>
       </c>
       <c r="M96" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N96">
         <v>0.1</v>
@@ -5585,7 +5588,7 @@
         <v>0.7</v>
       </c>
       <c r="P96">
-        <v>0.35</v>
+        <v>0.35000000000000003</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
@@ -5603,20 +5606,20 @@
         <v>364</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G97" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K97" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L97">
         <v>3</v>
       </c>
       <c r="M97" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N97">
         <v>0.05</v>
@@ -5625,7 +5628,7 @@
         <v>0.35</v>
       </c>
       <c r="P97">
-        <v>0.17499999999999999</v>
+        <v>0.17500000000000002</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
@@ -5643,20 +5646,20 @@
         <v>145.6</v>
       </c>
       <c r="F98" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G98" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K98" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L98">
         <v>3</v>
       </c>
       <c r="M98" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N98">
         <v>0.02</v>
@@ -5683,20 +5686,20 @@
         <v>72.8</v>
       </c>
       <c r="F99" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G99" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K99" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L99">
         <v>3</v>
       </c>
       <c r="M99" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N99">
         <v>0.01</v>
@@ -5723,20 +5726,20 @@
         <v>36.799999999999997</v>
       </c>
       <c r="F100" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G100" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K100" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L100">
         <v>3</v>
       </c>
       <c r="M100" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N100">
         <v>5.0000000000000001E-3</v>
@@ -5763,20 +5766,20 @@
         <v>15.44</v>
       </c>
       <c r="F101" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G101" s="10" t="str">
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
       <c r="K101" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L101">
         <v>3</v>
       </c>
       <c r="M101" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N101">
         <v>2E-3</v>
@@ -5790,7 +5793,7 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -5814,20 +5817,20 @@
         <v>36.4</v>
       </c>
       <c r="F103" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G103" s="10" t="str">
         <f t="shared" ref="G103:G113" si="7">IF(ISBLANK(D103),"Not Done",IF(AND(D103&lt;=E103,D103&gt;=C103),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
       <c r="K103" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L103">
         <v>4</v>
       </c>
       <c r="M103" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N103">
         <v>5</v>
@@ -5854,20 +5857,20 @@
         <v>14.56</v>
       </c>
       <c r="F104" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G104" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K104" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L104">
         <v>4</v>
       </c>
       <c r="M104" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N104">
         <v>2</v>
@@ -5894,20 +5897,20 @@
         <v>7.28</v>
       </c>
       <c r="F105" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G105" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K105" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L105">
         <v>4</v>
       </c>
       <c r="M105" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N105">
         <v>1</v>
@@ -5934,20 +5937,20 @@
         <v>3.64</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G106" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K106" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L106">
         <v>4</v>
       </c>
       <c r="M106" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N106">
         <v>0.5</v>
@@ -5974,20 +5977,20 @@
         <v>1.456</v>
       </c>
       <c r="F107" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G107" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K107" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L107">
         <v>4</v>
       </c>
       <c r="M107" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N107">
         <v>0.2</v>
@@ -6014,20 +6017,20 @@
         <v>728</v>
       </c>
       <c r="F108" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G108" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K108" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L108">
         <v>4</v>
       </c>
       <c r="M108" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N108">
         <v>0.1</v>
@@ -6036,7 +6039,7 @@
         <v>0.7</v>
       </c>
       <c r="P108">
-        <v>0.35</v>
+        <v>0.35000000000000003</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
@@ -6054,20 +6057,20 @@
         <v>364</v>
       </c>
       <c r="F109" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G109" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K109" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L109">
         <v>4</v>
       </c>
       <c r="M109" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N109">
         <v>0.05</v>
@@ -6076,7 +6079,7 @@
         <v>0.35</v>
       </c>
       <c r="P109">
-        <v>0.17499999999999999</v>
+        <v>0.17500000000000002</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
@@ -6094,20 +6097,20 @@
         <v>145</v>
       </c>
       <c r="F110" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G110" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K110" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L110">
         <v>4</v>
       </c>
       <c r="M110" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N110">
         <v>0.02</v>
@@ -6134,20 +6137,20 @@
         <v>72.8</v>
       </c>
       <c r="F111" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G111" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K111" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L111">
         <v>4</v>
       </c>
       <c r="M111" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N111">
         <v>0.01</v>
@@ -6174,20 +6177,20 @@
         <v>36.799999999999997</v>
       </c>
       <c r="F112" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G112" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K112" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L112">
         <v>4</v>
       </c>
       <c r="M112" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N112">
         <v>5.0000000000000001E-3</v>
@@ -6214,20 +6217,20 @@
         <v>15.44</v>
       </c>
       <c r="F113" s="10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="G113" s="10" t="str">
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
       <c r="K113" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="L113">
         <v>4</v>
       </c>
       <c r="M113" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="N113">
         <v>2E-3</v>
@@ -6239,34 +6242,34 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="116" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D116" s="12" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E116" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F116" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="F116" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B117" s="10"/>
       <c r="C117" s="13">
@@ -6277,7 +6280,7 @@
         <v>Not Done</v>
       </c>
       <c r="E117" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F117" s="10" t="str">
         <f>IF(ISBLANK(B117),"Not Done",IF(B117&lt;=C117,"Pass","Fail"))</f>
@@ -6293,14 +6296,14 @@
         <v>350</v>
       </c>
       <c r="D118" s="16" t="str">
-        <f>IFERROR((350/B118),"Not Done")</f>
+        <f t="shared" ref="D118:D120" si="8">IFERROR((350/B118),"Not Done")</f>
         <v>Not Done</v>
       </c>
       <c r="E118" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F118" s="10" t="str">
-        <f>IF(ISBLANK(B118),"Not Done",IF(B118&gt;=C118,"Pass","Fail"))</f>
+        <f t="shared" ref="F118:F120" si="9">IF(ISBLANK(B118),"Not Done",IF(B118&gt;=C118,"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
     </row>
@@ -6313,14 +6316,14 @@
         <v>350</v>
       </c>
       <c r="D119" s="16" t="str">
-        <f>IFERROR((350/B119),"Not Done")</f>
+        <f t="shared" si="8"/>
         <v>Not Done</v>
       </c>
       <c r="E119" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F119" s="10" t="str">
-        <f>IF(ISBLANK(B119),"Not Done",IF(B119&gt;=C119,"Pass","Fail"))</f>
+        <f t="shared" si="9"/>
         <v>Not Done</v>
       </c>
     </row>
@@ -6333,37 +6336,43 @@
         <v>350</v>
       </c>
       <c r="D120" s="16" t="str">
-        <f>IFERROR((350/B120),"Not Done")</f>
+        <f t="shared" si="8"/>
         <v>Not Done</v>
       </c>
       <c r="E120" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F120" s="10" t="str">
-        <f>IF(ISBLANK(B120),"Not Done",IF(B120&gt;=C120,"Pass","Fail"))</f>
-        <v>Not Done</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="9"/>
+        <v>Not Done</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="123" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="123" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D123" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E123" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E123" s="5" t="s">
-        <v>30</v>
+      <c r="K123" t="s">
+        <v>61</v>
+      </c>
+      <c r="L123" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
@@ -6375,41 +6384,44 @@
       </c>
       <c r="D124" s="10"/>
       <c r="E124" s="10" t="str">
-        <f>IF(ISBLANK(B124),"Not Done",IF(B124&lt;=C124,"Pass","Fail"))</f>
+        <f>IF(ISBLANK(B124),"Not Done",IF(ABS(B124)&lt;=C124,"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
       <c r="K124" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="126" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="L124">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
@@ -6419,28 +6431,28 @@
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C129" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D129" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="E129" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F129" s="10"/>
       <c r="J129" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
@@ -6450,49 +6462,49 @@
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B131" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C131" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D131" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="E131" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F131" s="10"/>
       <c r="J131" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="10" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B132" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="C132" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D132" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="E132" s="10" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F132" s="10"/>
       <c r="J132" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C134" s="14" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -7804,5 +7816,6 @@
     <brk id="63" max="6" man="1"/>
     <brk id="114" max="6" man="1"/>
   </rowBreaks>
+  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update test sheets for new templates
</commit_message>
<xml_diff>
--- a/testsheets/666_Keysight_DSOX3034A.xlsx
+++ b/testsheets/666_Keysight_DSOX3034A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Python\oscilloscope\testsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7C02ADB-7EE2-4BA2-AE92-49A9DE612135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C244BE56-5784-45A9-8F98-74F8C6A99003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="78">
   <si>
     <t>DSOX3034A</t>
   </si>
@@ -252,9 +252,6 @@
     <t>TRIG</t>
   </si>
   <si>
-    <t>AC</t>
-  </si>
-  <si>
     <t>Frequency</t>
   </si>
   <si>
@@ -269,15 +266,26 @@
   <si>
     <t>RISE</t>
   </si>
+  <si>
+    <t>Bandwidth</t>
+  </si>
+  <si>
+    <t>Invert</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="#\ &quot;V&quot;"/>
     <numFmt numFmtId="166" formatCode="#\ &quot;mV&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00&quot; ns&quot;"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -291,28 +299,33 @@
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -410,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -447,9 +460,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,6 +467,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2385,9 +2401,9 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A3:R136"/>
+  <dimension ref="A3:S136"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2399,18 +2415,18 @@
     <col min="6" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -2420,7 +2436,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -2434,7 +2450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2446,7 +2462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -2458,7 +2474,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2470,7 +2486,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -2484,7 +2500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2492,12 +2508,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
@@ -2519,30 +2535,35 @@
       <c r="G14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="M14" s="19" t="s">
+      <c r="M14" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="N14" s="19" t="s">
+      <c r="N14" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="O14" s="19" t="s">
+      <c r="O14" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="P14" s="19" t="s">
+      <c r="P14" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="Q14" s="19" t="s">
+      <c r="Q14" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="R14" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="R14" s="19"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>29</v>
       </c>
@@ -2552,16 +2573,16 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>5</v>
       </c>
@@ -2582,26 +2603,26 @@
         <f t="shared" ref="G16:G26" si="0">IF(ISBLANK(D16),"Not Done",IF(AND(D16&lt;=E16,D16&gt;=C16),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L16" s="19">
+      <c r="L16" s="18">
         <v>1</v>
       </c>
-      <c r="M16" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N16" s="19">
+      <c r="M16" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" s="18">
         <v>5</v>
       </c>
-      <c r="O16" s="19">
+      <c r="O16" s="18">
         <v>35</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="18">
         <v>17.5</v>
       </c>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
@@ -2624,26 +2645,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="18">
         <v>1</v>
       </c>
-      <c r="M17" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N17" s="19">
+      <c r="M17" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="18">
         <v>2</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="18">
         <v>14</v>
       </c>
-      <c r="P17" s="19">
+      <c r="P17" s="18">
         <v>7</v>
       </c>
-      <c r="Q17" s="19"/>
-      <c r="R17" s="19"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
@@ -2666,26 +2687,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="K18" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="18">
         <v>1</v>
       </c>
-      <c r="M18" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N18" s="19">
+      <c r="M18" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N18" s="18">
         <v>1</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="18">
         <v>7</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="18">
         <v>3.5</v>
       </c>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="19"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
@@ -2708,26 +2729,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L19" s="19">
+      <c r="L19" s="18">
         <v>1</v>
       </c>
-      <c r="M19" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N19" s="19">
+      <c r="M19" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" s="18">
         <v>0.5</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="18">
         <v>3.5</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="18">
         <v>1.75</v>
       </c>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="19"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
@@ -2750,26 +2771,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K20" s="19" t="s">
+      <c r="K20" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L20" s="19">
+      <c r="L20" s="18">
         <v>1</v>
       </c>
-      <c r="M20" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N20" s="19">
+      <c r="M20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" s="18">
         <v>0.2</v>
       </c>
-      <c r="O20" s="19">
+      <c r="O20" s="18">
         <v>1.4</v>
       </c>
-      <c r="P20" s="19">
+      <c r="P20" s="18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
@@ -2792,26 +2813,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K21" s="19" t="s">
+      <c r="K21" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L21" s="19">
+      <c r="L21" s="18">
         <v>1</v>
       </c>
-      <c r="M21" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N21" s="19">
+      <c r="M21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21" s="18">
         <v>0.1</v>
       </c>
-      <c r="O21" s="19">
+      <c r="O21" s="18">
         <v>0.7</v>
       </c>
-      <c r="P21" s="19">
+      <c r="P21" s="18">
         <v>0.35000000000000003</v>
       </c>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="19"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
@@ -2834,26 +2855,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="K22" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L22" s="19">
+      <c r="L22" s="18">
         <v>1</v>
       </c>
-      <c r="M22" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N22" s="19">
+      <c r="M22" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N22" s="18">
         <v>0.05</v>
       </c>
-      <c r="O22" s="19">
+      <c r="O22" s="18">
         <v>0.35</v>
       </c>
-      <c r="P22" s="19">
+      <c r="P22" s="18">
         <v>0.17500000000000002</v>
       </c>
-      <c r="Q22" s="19"/>
-      <c r="R22" s="19"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
@@ -2876,26 +2897,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K23" s="19" t="s">
+      <c r="K23" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L23" s="19">
+      <c r="L23" s="18">
         <v>1</v>
       </c>
-      <c r="M23" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N23" s="19">
+      <c r="M23" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="18">
         <v>0.02</v>
       </c>
-      <c r="O23" s="19">
+      <c r="O23" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P23" s="19">
+      <c r="P23" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
@@ -2918,26 +2939,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K24" s="19" t="s">
+      <c r="K24" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L24" s="19">
+      <c r="L24" s="18">
         <v>1</v>
       </c>
-      <c r="M24" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N24" s="19">
+      <c r="M24" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N24" s="18">
         <v>0.01</v>
       </c>
-      <c r="O24" s="19">
+      <c r="O24" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P24" s="19">
+      <c r="P24" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
@@ -2960,26 +2981,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K25" s="19" t="s">
+      <c r="K25" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L25" s="19">
+      <c r="L25" s="18">
         <v>1</v>
       </c>
-      <c r="M25" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N25" s="19">
+      <c r="M25" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O25" s="19">
+      <c r="O25" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P25" s="19">
+      <c r="P25" s="18">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="Q25" s="19"/>
-      <c r="R25" s="19"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
@@ -3002,26 +3023,26 @@
         <f t="shared" si="0"/>
         <v>Not Done</v>
       </c>
-      <c r="K26" s="19" t="s">
+      <c r="K26" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L26" s="19">
+      <c r="L26" s="18">
         <v>1</v>
       </c>
-      <c r="M26" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N26" s="19">
+      <c r="M26" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N26" s="18">
         <v>2E-3</v>
       </c>
-      <c r="O26" s="19">
+      <c r="O26" s="18">
         <v>1.4E-2</v>
       </c>
-      <c r="P26" s="19">
+      <c r="P26" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="Q26" s="19"/>
-      <c r="R26" s="19"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
@@ -3033,14 +3054,14 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
@@ -3063,26 +3084,26 @@
         <f t="shared" ref="G28:G38" si="1">IF(ISBLANK(D28),"Not Done",IF(AND(D28&lt;=E28,D28&gt;=C28),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L28" s="19">
+      <c r="L28" s="18">
         <v>2</v>
       </c>
-      <c r="M28" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N28" s="19">
+      <c r="M28" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N28" s="18">
         <v>5</v>
       </c>
-      <c r="O28" s="19">
+      <c r="O28" s="18">
         <v>35</v>
       </c>
-      <c r="P28" s="19">
+      <c r="P28" s="18">
         <v>17.5</v>
       </c>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
@@ -3105,26 +3126,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K29" s="19" t="s">
+      <c r="K29" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L29" s="19">
+      <c r="L29" s="18">
         <v>2</v>
       </c>
-      <c r="M29" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N29" s="19">
+      <c r="M29" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N29" s="18">
         <v>2</v>
       </c>
-      <c r="O29" s="19">
+      <c r="O29" s="18">
         <v>14</v>
       </c>
-      <c r="P29" s="19">
+      <c r="P29" s="18">
         <v>7</v>
       </c>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="19"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
@@ -3147,26 +3168,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K30" s="19" t="s">
+      <c r="K30" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L30" s="19">
+      <c r="L30" s="18">
         <v>2</v>
       </c>
-      <c r="M30" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N30" s="19">
+      <c r="M30" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="18">
         <v>1</v>
       </c>
-      <c r="O30" s="19">
+      <c r="O30" s="18">
         <v>7</v>
       </c>
-      <c r="P30" s="19">
+      <c r="P30" s="18">
         <v>3.5</v>
       </c>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
@@ -3189,26 +3210,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K31" s="19" t="s">
+      <c r="K31" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L31" s="19">
+      <c r="L31" s="18">
         <v>2</v>
       </c>
-      <c r="M31" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N31" s="19">
+      <c r="M31" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N31" s="18">
         <v>0.5</v>
       </c>
-      <c r="O31" s="19">
+      <c r="O31" s="18">
         <v>3.5</v>
       </c>
-      <c r="P31" s="19">
+      <c r="P31" s="18">
         <v>1.75</v>
       </c>
-      <c r="Q31" s="19"/>
-      <c r="R31" s="19"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="18"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
@@ -3231,26 +3252,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K32" s="19" t="s">
+      <c r="K32" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L32" s="19">
+      <c r="L32" s="18">
         <v>2</v>
       </c>
-      <c r="M32" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N32" s="19">
+      <c r="M32" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N32" s="18">
         <v>0.2</v>
       </c>
-      <c r="O32" s="19">
+      <c r="O32" s="18">
         <v>1.4</v>
       </c>
-      <c r="P32" s="19">
+      <c r="P32" s="18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="Q32" s="19"/>
-      <c r="R32" s="19"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
@@ -3273,26 +3294,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K33" s="19" t="s">
+      <c r="K33" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L33" s="19">
+      <c r="L33" s="18">
         <v>2</v>
       </c>
-      <c r="M33" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N33" s="19">
+      <c r="M33" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N33" s="18">
         <v>0.1</v>
       </c>
-      <c r="O33" s="19">
+      <c r="O33" s="18">
         <v>0.7</v>
       </c>
-      <c r="P33" s="19">
+      <c r="P33" s="18">
         <v>0.35000000000000003</v>
       </c>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
+      <c r="Q33" s="18"/>
+      <c r="R33" s="18"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
@@ -3315,26 +3336,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K34" s="19" t="s">
+      <c r="K34" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L34" s="19">
+      <c r="L34" s="18">
         <v>2</v>
       </c>
-      <c r="M34" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N34" s="19">
+      <c r="M34" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N34" s="18">
         <v>0.05</v>
       </c>
-      <c r="O34" s="19">
+      <c r="O34" s="18">
         <v>0.35</v>
       </c>
-      <c r="P34" s="19">
+      <c r="P34" s="18">
         <v>0.17500000000000002</v>
       </c>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
@@ -3357,26 +3378,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K35" s="19" t="s">
+      <c r="K35" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L35" s="19">
+      <c r="L35" s="18">
         <v>2</v>
       </c>
-      <c r="M35" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N35" s="19">
+      <c r="M35" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N35" s="18">
         <v>0.02</v>
       </c>
-      <c r="O35" s="19">
+      <c r="O35" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P35" s="19">
+      <c r="P35" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="19"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
@@ -3399,26 +3420,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K36" s="19" t="s">
+      <c r="K36" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L36" s="19">
+      <c r="L36" s="18">
         <v>2</v>
       </c>
-      <c r="M36" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N36" s="19">
+      <c r="M36" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N36" s="18">
         <v>0.01</v>
       </c>
-      <c r="O36" s="19">
+      <c r="O36" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P36" s="19">
+      <c r="P36" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
+      <c r="Q36" s="18"/>
+      <c r="R36" s="18"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
@@ -3441,26 +3462,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K37" s="19" t="s">
+      <c r="K37" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L37" s="19">
+      <c r="L37" s="18">
         <v>2</v>
       </c>
-      <c r="M37" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N37" s="19">
+      <c r="M37" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N37" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O37" s="19">
+      <c r="O37" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P37" s="19">
+      <c r="P37" s="18">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="Q37" s="19"/>
-      <c r="R37" s="19"/>
+      <c r="Q37" s="18"/>
+      <c r="R37" s="18"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
@@ -3483,26 +3504,26 @@
         <f t="shared" si="1"/>
         <v>Not Done</v>
       </c>
-      <c r="K38" s="19" t="s">
+      <c r="K38" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L38" s="19">
+      <c r="L38" s="18">
         <v>2</v>
       </c>
-      <c r="M38" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N38" s="19">
+      <c r="M38" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N38" s="18">
         <v>2E-3</v>
       </c>
-      <c r="O38" s="19">
+      <c r="O38" s="18">
         <v>1.4E-2</v>
       </c>
-      <c r="P38" s="19">
+      <c r="P38" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="Q38" s="19"/>
-      <c r="R38" s="19"/>
+      <c r="Q38" s="18"/>
+      <c r="R38" s="18"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
@@ -3514,14 +3535,14 @@
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="19"/>
-      <c r="R39" s="19"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
@@ -3544,26 +3565,26 @@
         <f t="shared" ref="G40:G50" si="2">IF(ISBLANK(D40),"Not Done",IF(AND(D40&lt;=E40,D40&gt;=C40),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="K40" s="19" t="s">
+      <c r="K40" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L40" s="19">
+      <c r="L40" s="18">
         <v>3</v>
       </c>
-      <c r="M40" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N40" s="19">
+      <c r="M40" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N40" s="18">
         <v>5</v>
       </c>
-      <c r="O40" s="19">
+      <c r="O40" s="18">
         <v>35</v>
       </c>
-      <c r="P40" s="19">
+      <c r="P40" s="18">
         <v>17.5</v>
       </c>
-      <c r="Q40" s="19"/>
-      <c r="R40" s="19"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
@@ -3586,26 +3607,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K41" s="19" t="s">
+      <c r="K41" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L41" s="19">
+      <c r="L41" s="18">
         <v>3</v>
       </c>
-      <c r="M41" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N41" s="19">
+      <c r="M41" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N41" s="18">
         <v>2</v>
       </c>
-      <c r="O41" s="19">
+      <c r="O41" s="18">
         <v>14</v>
       </c>
-      <c r="P41" s="19">
+      <c r="P41" s="18">
         <v>7</v>
       </c>
-      <c r="Q41" s="19"/>
-      <c r="R41" s="19"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
@@ -3628,26 +3649,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K42" s="19" t="s">
+      <c r="K42" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L42" s="19">
+      <c r="L42" s="18">
         <v>3</v>
       </c>
-      <c r="M42" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N42" s="19">
+      <c r="M42" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N42" s="18">
         <v>1</v>
       </c>
-      <c r="O42" s="19">
+      <c r="O42" s="18">
         <v>7</v>
       </c>
-      <c r="P42" s="19">
+      <c r="P42" s="18">
         <v>3.5</v>
       </c>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
@@ -3670,26 +3691,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K43" s="19" t="s">
+      <c r="K43" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L43" s="19">
+      <c r="L43" s="18">
         <v>3</v>
       </c>
-      <c r="M43" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N43" s="19">
+      <c r="M43" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N43" s="18">
         <v>0.5</v>
       </c>
-      <c r="O43" s="19">
+      <c r="O43" s="18">
         <v>3.5</v>
       </c>
-      <c r="P43" s="19">
+      <c r="P43" s="18">
         <v>1.75</v>
       </c>
-      <c r="Q43" s="19"/>
-      <c r="R43" s="19"/>
+      <c r="Q43" s="18"/>
+      <c r="R43" s="18"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="11">
@@ -3712,26 +3733,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K44" s="19" t="s">
+      <c r="K44" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L44" s="19">
+      <c r="L44" s="18">
         <v>3</v>
       </c>
-      <c r="M44" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N44" s="19">
+      <c r="M44" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N44" s="18">
         <v>0.2</v>
       </c>
-      <c r="O44" s="19">
+      <c r="O44" s="18">
         <v>1.4</v>
       </c>
-      <c r="P44" s="19">
+      <c r="P44" s="18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="Q44" s="19"/>
-      <c r="R44" s="19"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="11">
@@ -3754,26 +3775,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K45" s="19" t="s">
+      <c r="K45" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L45" s="19">
+      <c r="L45" s="18">
         <v>3</v>
       </c>
-      <c r="M45" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N45" s="19">
+      <c r="M45" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N45" s="18">
         <v>0.1</v>
       </c>
-      <c r="O45" s="19">
+      <c r="O45" s="18">
         <v>0.7</v>
       </c>
-      <c r="P45" s="19">
+      <c r="P45" s="18">
         <v>0.35000000000000003</v>
       </c>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="11">
@@ -3796,26 +3817,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K46" s="19" t="s">
+      <c r="K46" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L46" s="19">
+      <c r="L46" s="18">
         <v>3</v>
       </c>
-      <c r="M46" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N46" s="19">
+      <c r="M46" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N46" s="18">
         <v>0.05</v>
       </c>
-      <c r="O46" s="19">
+      <c r="O46" s="18">
         <v>0.35</v>
       </c>
-      <c r="P46" s="19">
+      <c r="P46" s="18">
         <v>0.17500000000000002</v>
       </c>
-      <c r="Q46" s="19"/>
-      <c r="R46" s="19"/>
+      <c r="Q46" s="18"/>
+      <c r="R46" s="18"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="11">
@@ -3838,26 +3859,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K47" s="19" t="s">
+      <c r="K47" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L47" s="19">
+      <c r="L47" s="18">
         <v>3</v>
       </c>
-      <c r="M47" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N47" s="19">
+      <c r="M47" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N47" s="18">
         <v>0.02</v>
       </c>
-      <c r="O47" s="19">
+      <c r="O47" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P47" s="19">
+      <c r="P47" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q47" s="19"/>
-      <c r="R47" s="19"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="11">
@@ -3880,26 +3901,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K48" s="19" t="s">
+      <c r="K48" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L48" s="19">
+      <c r="L48" s="18">
         <v>3</v>
       </c>
-      <c r="M48" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N48" s="19">
+      <c r="M48" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N48" s="18">
         <v>0.01</v>
       </c>
-      <c r="O48" s="19">
+      <c r="O48" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P48" s="19">
+      <c r="P48" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q48" s="19"/>
-      <c r="R48" s="19"/>
+      <c r="Q48" s="18"/>
+      <c r="R48" s="18"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="11">
@@ -3922,26 +3943,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K49" s="19" t="s">
+      <c r="K49" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L49" s="19">
+      <c r="L49" s="18">
         <v>3</v>
       </c>
-      <c r="M49" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N49" s="19">
+      <c r="M49" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N49" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O49" s="19">
+      <c r="O49" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P49" s="19">
+      <c r="P49" s="18">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="Q49" s="19"/>
-      <c r="R49" s="19"/>
+      <c r="Q49" s="18"/>
+      <c r="R49" s="18"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="11">
@@ -3964,26 +3985,26 @@
         <f t="shared" si="2"/>
         <v>Not Done</v>
       </c>
-      <c r="K50" s="19" t="s">
+      <c r="K50" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L50" s="19">
+      <c r="L50" s="18">
         <v>3</v>
       </c>
-      <c r="M50" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N50" s="19">
+      <c r="M50" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N50" s="18">
         <v>2E-3</v>
       </c>
-      <c r="O50" s="19">
+      <c r="O50" s="18">
         <v>1.4E-2</v>
       </c>
-      <c r="P50" s="19">
+      <c r="P50" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="Q50" s="19"/>
-      <c r="R50" s="19"/>
+      <c r="Q50" s="18"/>
+      <c r="R50" s="18"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
@@ -3995,14 +4016,14 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="19"/>
-      <c r="M51" s="19"/>
-      <c r="N51" s="19"/>
-      <c r="O51" s="19"/>
-      <c r="P51" s="19"/>
-      <c r="Q51" s="19"/>
-      <c r="R51" s="19"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18"/>
+      <c r="Q51" s="18"/>
+      <c r="R51" s="18"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
@@ -4025,26 +4046,26 @@
         <f t="shared" ref="G52:G62" si="3">IF(ISBLANK(D52),"Not Done",IF(AND(D52&lt;=E52,D52&gt;=C52),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="K52" s="19" t="s">
+      <c r="K52" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L52" s="19">
+      <c r="L52" s="18">
         <v>4</v>
       </c>
-      <c r="M52" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N52" s="19">
+      <c r="M52" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N52" s="18">
         <v>5</v>
       </c>
-      <c r="O52" s="19">
+      <c r="O52" s="18">
         <v>35</v>
       </c>
-      <c r="P52" s="19">
+      <c r="P52" s="18">
         <v>17.5</v>
       </c>
-      <c r="Q52" s="19"/>
-      <c r="R52" s="19"/>
+      <c r="Q52" s="18"/>
+      <c r="R52" s="18"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
@@ -4067,26 +4088,26 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K53" s="19" t="s">
+      <c r="K53" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L53" s="19">
+      <c r="L53" s="18">
         <v>4</v>
       </c>
-      <c r="M53" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N53" s="19">
+      <c r="M53" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N53" s="18">
         <v>2</v>
       </c>
-      <c r="O53" s="19">
+      <c r="O53" s="18">
         <v>14</v>
       </c>
-      <c r="P53" s="19">
+      <c r="P53" s="18">
         <v>7</v>
       </c>
-      <c r="Q53" s="19"/>
-      <c r="R53" s="19"/>
+      <c r="Q53" s="18"/>
+      <c r="R53" s="18"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
@@ -4109,26 +4130,26 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K54" s="19" t="s">
+      <c r="K54" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L54" s="19">
+      <c r="L54" s="18">
         <v>4</v>
       </c>
-      <c r="M54" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N54" s="19">
+      <c r="M54" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N54" s="18">
         <v>1</v>
       </c>
-      <c r="O54" s="19">
+      <c r="O54" s="18">
         <v>7</v>
       </c>
-      <c r="P54" s="19">
+      <c r="P54" s="18">
         <v>3.5</v>
       </c>
-      <c r="Q54" s="19"/>
-      <c r="R54" s="19"/>
+      <c r="Q54" s="18"/>
+      <c r="R54" s="18"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="11">
@@ -4151,26 +4172,26 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K55" s="19" t="s">
+      <c r="K55" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L55" s="19">
+      <c r="L55" s="18">
         <v>4</v>
       </c>
-      <c r="M55" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N55" s="19">
+      <c r="M55" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N55" s="18">
         <v>0.5</v>
       </c>
-      <c r="O55" s="19">
+      <c r="O55" s="18">
         <v>3.5</v>
       </c>
-      <c r="P55" s="19">
+      <c r="P55" s="18">
         <v>1.75</v>
       </c>
-      <c r="Q55" s="19"/>
-      <c r="R55" s="19"/>
+      <c r="Q55" s="18"/>
+      <c r="R55" s="18"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="11">
@@ -4193,26 +4214,26 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K56" s="19" t="s">
+      <c r="K56" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L56" s="19">
+      <c r="L56" s="18">
         <v>4</v>
       </c>
-      <c r="M56" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N56" s="19">
+      <c r="M56" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N56" s="18">
         <v>0.2</v>
       </c>
-      <c r="O56" s="19">
+      <c r="O56" s="18">
         <v>1.4</v>
       </c>
-      <c r="P56" s="19">
+      <c r="P56" s="18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="Q56" s="19"/>
-      <c r="R56" s="19"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" s="18"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="11">
@@ -4235,26 +4256,26 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K57" s="19" t="s">
+      <c r="K57" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L57" s="19">
+      <c r="L57" s="18">
         <v>4</v>
       </c>
-      <c r="M57" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N57" s="19">
+      <c r="M57" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N57" s="18">
         <v>0.1</v>
       </c>
-      <c r="O57" s="19">
+      <c r="O57" s="18">
         <v>0.7</v>
       </c>
-      <c r="P57" s="19">
+      <c r="P57" s="18">
         <v>0.35000000000000003</v>
       </c>
-      <c r="Q57" s="19"/>
-      <c r="R57" s="19"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="11">
@@ -4277,26 +4298,26 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K58" s="19" t="s">
+      <c r="K58" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L58" s="19">
+      <c r="L58" s="18">
         <v>4</v>
       </c>
-      <c r="M58" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N58" s="19">
+      <c r="M58" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N58" s="18">
         <v>0.05</v>
       </c>
-      <c r="O58" s="19">
+      <c r="O58" s="18">
         <v>0.35</v>
       </c>
-      <c r="P58" s="19">
+      <c r="P58" s="18">
         <v>0.17500000000000002</v>
       </c>
-      <c r="Q58" s="19"/>
-      <c r="R58" s="19"/>
+      <c r="Q58" s="18"/>
+      <c r="R58" s="18"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="11">
@@ -4319,26 +4340,26 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K59" s="19" t="s">
+      <c r="K59" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L59" s="19">
+      <c r="L59" s="18">
         <v>4</v>
       </c>
-      <c r="M59" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N59" s="19">
+      <c r="M59" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N59" s="18">
         <v>0.02</v>
       </c>
-      <c r="O59" s="19">
+      <c r="O59" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P59" s="19">
+      <c r="P59" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q59" s="19"/>
-      <c r="R59" s="19"/>
+      <c r="Q59" s="18"/>
+      <c r="R59" s="18"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="11">
@@ -4361,26 +4382,26 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K60" s="19" t="s">
+      <c r="K60" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L60" s="19">
+      <c r="L60" s="18">
         <v>4</v>
       </c>
-      <c r="M60" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N60" s="19">
+      <c r="M60" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N60" s="18">
         <v>0.01</v>
       </c>
-      <c r="O60" s="19">
+      <c r="O60" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P60" s="19">
+      <c r="P60" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q60" s="19"/>
-      <c r="R60" s="19"/>
+      <c r="Q60" s="18"/>
+      <c r="R60" s="18"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
@@ -4403,26 +4424,26 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K61" s="19" t="s">
+      <c r="K61" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L61" s="19">
+      <c r="L61" s="18">
         <v>4</v>
       </c>
-      <c r="M61" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N61" s="19">
+      <c r="M61" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N61" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O61" s="19">
+      <c r="O61" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P61" s="19">
+      <c r="P61" s="18">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="Q61" s="19"/>
-      <c r="R61" s="19"/>
+      <c r="Q61" s="18"/>
+      <c r="R61" s="18"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
@@ -4445,49 +4466,49 @@
         <f t="shared" si="3"/>
         <v>Not Done</v>
       </c>
-      <c r="K62" s="19" t="s">
+      <c r="K62" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="L62" s="19">
+      <c r="L62" s="18">
         <v>4</v>
       </c>
-      <c r="M62" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N62" s="19">
+      <c r="M62" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N62" s="18">
         <v>2E-3</v>
       </c>
-      <c r="O62" s="19">
+      <c r="O62" s="18">
         <v>1.4E-2</v>
       </c>
-      <c r="P62" s="19">
+      <c r="P62" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="Q62" s="19"/>
-      <c r="R62" s="19"/>
+      <c r="Q62" s="18"/>
+      <c r="R62" s="18"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K63" s="19"/>
-      <c r="L63" s="19"/>
-      <c r="M63" s="19"/>
-      <c r="N63" s="19"/>
-      <c r="O63" s="19"/>
-      <c r="P63" s="19"/>
-      <c r="Q63" s="19"/>
-      <c r="R63" s="19"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="18"/>
+      <c r="M63" s="18"/>
+      <c r="N63" s="18"/>
+      <c r="O63" s="18"/>
+      <c r="P63" s="18"/>
+      <c r="Q63" s="18"/>
+      <c r="R63" s="18"/>
     </row>
     <row r="64" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K64" s="19"/>
-      <c r="L64" s="19"/>
-      <c r="M64" s="19"/>
-      <c r="N64" s="19"/>
-      <c r="O64" s="19"/>
-      <c r="P64" s="19"/>
-      <c r="Q64" s="19"/>
-      <c r="R64" s="19"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
+      <c r="M64" s="18"/>
+      <c r="N64" s="18"/>
+      <c r="O64" s="18"/>
+      <c r="P64" s="18"/>
+      <c r="Q64" s="18"/>
+      <c r="R64" s="18"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
@@ -4511,14 +4532,14 @@
       <c r="G65" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K65" s="19"/>
-      <c r="L65" s="19"/>
-      <c r="M65" s="19"/>
-      <c r="N65" s="19"/>
-      <c r="O65" s="19"/>
-      <c r="P65" s="19"/>
-      <c r="Q65" s="19"/>
-      <c r="R65" s="19"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="18"/>
+      <c r="Q65" s="18"/>
+      <c r="R65" s="18"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
@@ -4530,14 +4551,14 @@
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
-      <c r="K66" s="19"/>
-      <c r="L66" s="19"/>
-      <c r="M66" s="19"/>
-      <c r="N66" s="19"/>
-      <c r="O66" s="19"/>
-      <c r="P66" s="19"/>
-      <c r="Q66" s="19"/>
-      <c r="R66" s="19"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+      <c r="M66" s="18"/>
+      <c r="N66" s="18"/>
+      <c r="O66" s="18"/>
+      <c r="P66" s="18"/>
+      <c r="Q66" s="18"/>
+      <c r="R66" s="18"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
@@ -4560,26 +4581,26 @@
         <f t="shared" ref="G67:G77" si="4">IF(ISBLANK(D67),"Not Done",IF(AND(D67&lt;=E67,D67&gt;=C67),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="K67" s="19" t="s">
+      <c r="K67" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L67" s="19">
+      <c r="L67" s="18">
         <v>1</v>
       </c>
-      <c r="M67" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N67" s="19">
+      <c r="M67" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N67" s="18">
         <v>5</v>
       </c>
-      <c r="O67" s="19">
+      <c r="O67" s="18">
         <v>35</v>
       </c>
-      <c r="P67" s="19">
+      <c r="P67" s="18">
         <v>17.5</v>
       </c>
-      <c r="Q67" s="19"/>
-      <c r="R67" s="19"/>
+      <c r="Q67" s="18"/>
+      <c r="R67" s="18"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
@@ -4602,26 +4623,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K68" s="19" t="s">
+      <c r="K68" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L68" s="19">
+      <c r="L68" s="18">
         <v>1</v>
       </c>
-      <c r="M68" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N68" s="19">
+      <c r="M68" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N68" s="18">
         <v>2</v>
       </c>
-      <c r="O68" s="19">
+      <c r="O68" s="18">
         <v>14</v>
       </c>
-      <c r="P68" s="19">
+      <c r="P68" s="18">
         <v>7</v>
       </c>
-      <c r="Q68" s="19"/>
-      <c r="R68" s="19"/>
+      <c r="Q68" s="18"/>
+      <c r="R68" s="18"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
@@ -4644,26 +4665,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K69" s="19" t="s">
+      <c r="K69" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L69" s="19">
+      <c r="L69" s="18">
         <v>1</v>
       </c>
-      <c r="M69" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N69" s="19">
+      <c r="M69" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N69" s="18">
         <v>1</v>
       </c>
-      <c r="O69" s="19">
+      <c r="O69" s="18">
         <v>7</v>
       </c>
-      <c r="P69" s="19">
+      <c r="P69" s="18">
         <v>3.5</v>
       </c>
-      <c r="Q69" s="19"/>
-      <c r="R69" s="19"/>
+      <c r="Q69" s="18"/>
+      <c r="R69" s="18"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="11">
@@ -4686,26 +4707,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K70" s="19" t="s">
+      <c r="K70" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L70" s="19">
+      <c r="L70" s="18">
         <v>1</v>
       </c>
-      <c r="M70" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N70" s="19">
+      <c r="M70" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N70" s="18">
         <v>0.5</v>
       </c>
-      <c r="O70" s="19">
+      <c r="O70" s="18">
         <v>3.5</v>
       </c>
-      <c r="P70" s="19">
+      <c r="P70" s="18">
         <v>1.75</v>
       </c>
-      <c r="Q70" s="19"/>
-      <c r="R70" s="19"/>
+      <c r="Q70" s="18"/>
+      <c r="R70" s="18"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="11">
@@ -4728,26 +4749,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K71" s="19" t="s">
+      <c r="K71" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L71" s="19">
+      <c r="L71" s="18">
         <v>1</v>
       </c>
-      <c r="M71" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N71" s="19">
+      <c r="M71" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N71" s="18">
         <v>0.2</v>
       </c>
-      <c r="O71" s="19">
+      <c r="O71" s="18">
         <v>1.4</v>
       </c>
-      <c r="P71" s="19">
+      <c r="P71" s="18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="Q71" s="19"/>
-      <c r="R71" s="19"/>
+      <c r="Q71" s="18"/>
+      <c r="R71" s="18"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
@@ -4770,26 +4791,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K72" s="19" t="s">
+      <c r="K72" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L72" s="19">
+      <c r="L72" s="18">
         <v>1</v>
       </c>
-      <c r="M72" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N72" s="19">
+      <c r="M72" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N72" s="18">
         <v>0.1</v>
       </c>
-      <c r="O72" s="19">
+      <c r="O72" s="18">
         <v>0.7</v>
       </c>
-      <c r="P72" s="19">
+      <c r="P72" s="18">
         <v>0.35000000000000003</v>
       </c>
-      <c r="Q72" s="19"/>
-      <c r="R72" s="19"/>
+      <c r="Q72" s="18"/>
+      <c r="R72" s="18"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="11">
@@ -4812,26 +4833,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K73" s="19" t="s">
+      <c r="K73" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L73" s="19">
+      <c r="L73" s="18">
         <v>1</v>
       </c>
-      <c r="M73" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N73" s="19">
+      <c r="M73" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N73" s="18">
         <v>0.05</v>
       </c>
-      <c r="O73" s="19">
+      <c r="O73" s="18">
         <v>0.35</v>
       </c>
-      <c r="P73" s="19">
+      <c r="P73" s="18">
         <v>0.17500000000000002</v>
       </c>
-      <c r="Q73" s="19"/>
-      <c r="R73" s="19"/>
+      <c r="Q73" s="18"/>
+      <c r="R73" s="18"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="11">
@@ -4854,26 +4875,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K74" s="19" t="s">
+      <c r="K74" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L74" s="19">
+      <c r="L74" s="18">
         <v>1</v>
       </c>
-      <c r="M74" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N74" s="19">
+      <c r="M74" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N74" s="18">
         <v>0.02</v>
       </c>
-      <c r="O74" s="19">
+      <c r="O74" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P74" s="19">
+      <c r="P74" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q74" s="19"/>
-      <c r="R74" s="19"/>
+      <c r="Q74" s="18"/>
+      <c r="R74" s="18"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="11">
@@ -4896,26 +4917,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K75" s="19" t="s">
+      <c r="K75" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L75" s="19">
+      <c r="L75" s="18">
         <v>1</v>
       </c>
-      <c r="M75" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N75" s="19">
+      <c r="M75" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N75" s="18">
         <v>0.01</v>
       </c>
-      <c r="O75" s="19">
+      <c r="O75" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P75" s="19">
+      <c r="P75" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q75" s="19"/>
-      <c r="R75" s="19"/>
+      <c r="Q75" s="18"/>
+      <c r="R75" s="18"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="11">
@@ -4938,26 +4959,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K76" s="19" t="s">
+      <c r="K76" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L76" s="19">
+      <c r="L76" s="18">
         <v>1</v>
       </c>
-      <c r="M76" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N76" s="19">
+      <c r="M76" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N76" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O76" s="19">
+      <c r="O76" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P76" s="19">
+      <c r="P76" s="18">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="Q76" s="19"/>
-      <c r="R76" s="19"/>
+      <c r="Q76" s="18"/>
+      <c r="R76" s="18"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="11">
@@ -4980,26 +5001,26 @@
         <f t="shared" si="4"/>
         <v>Not Done</v>
       </c>
-      <c r="K77" s="19" t="s">
+      <c r="K77" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L77" s="19">
+      <c r="L77" s="18">
         <v>1</v>
       </c>
-      <c r="M77" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N77" s="19">
+      <c r="M77" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N77" s="18">
         <v>2E-3</v>
       </c>
-      <c r="O77" s="19">
+      <c r="O77" s="18">
         <v>1.4E-2</v>
       </c>
-      <c r="P77" s="19">
+      <c r="P77" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="Q77" s="19"/>
-      <c r="R77" s="19"/>
+      <c r="Q77" s="18"/>
+      <c r="R77" s="18"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
@@ -5011,14 +5032,14 @@
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
-      <c r="K78" s="19"/>
-      <c r="L78" s="19"/>
-      <c r="M78" s="19"/>
-      <c r="N78" s="19"/>
-      <c r="O78" s="19"/>
-      <c r="P78" s="19"/>
-      <c r="Q78" s="19"/>
-      <c r="R78" s="19"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="18"/>
+      <c r="P78" s="18"/>
+      <c r="Q78" s="18"/>
+      <c r="R78" s="18"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
@@ -5041,26 +5062,26 @@
         <f t="shared" ref="G79:G89" si="5">IF(ISBLANK(D79),"Not Done",IF(AND(D79&lt;=E79,D79&gt;=C79),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="K79" s="19" t="s">
+      <c r="K79" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L79" s="19">
+      <c r="L79" s="18">
         <v>2</v>
       </c>
-      <c r="M79" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N79" s="19">
+      <c r="M79" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N79" s="18">
         <v>5</v>
       </c>
-      <c r="O79" s="19">
+      <c r="O79" s="18">
         <v>35</v>
       </c>
-      <c r="P79" s="19">
+      <c r="P79" s="18">
         <v>17.5</v>
       </c>
-      <c r="Q79" s="19"/>
-      <c r="R79" s="19"/>
+      <c r="Q79" s="18"/>
+      <c r="R79" s="18"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
@@ -5083,26 +5104,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K80" s="19" t="s">
+      <c r="K80" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L80" s="19">
+      <c r="L80" s="18">
         <v>2</v>
       </c>
-      <c r="M80" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N80" s="19">
+      <c r="M80" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N80" s="18">
         <v>2</v>
       </c>
-      <c r="O80" s="19">
+      <c r="O80" s="18">
         <v>14</v>
       </c>
-      <c r="P80" s="19">
+      <c r="P80" s="18">
         <v>7</v>
       </c>
-      <c r="Q80" s="19"/>
-      <c r="R80" s="19"/>
+      <c r="Q80" s="18"/>
+      <c r="R80" s="18"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
@@ -5125,26 +5146,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K81" s="19" t="s">
+      <c r="K81" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L81" s="19">
+      <c r="L81" s="18">
         <v>2</v>
       </c>
-      <c r="M81" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N81" s="19">
+      <c r="M81" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N81" s="18">
         <v>1</v>
       </c>
-      <c r="O81" s="19">
+      <c r="O81" s="18">
         <v>7</v>
       </c>
-      <c r="P81" s="19">
+      <c r="P81" s="18">
         <v>3.5</v>
       </c>
-      <c r="Q81" s="19"/>
-      <c r="R81" s="19"/>
+      <c r="Q81" s="18"/>
+      <c r="R81" s="18"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="11">
@@ -5167,26 +5188,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K82" s="19" t="s">
+      <c r="K82" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L82" s="19">
+      <c r="L82" s="18">
         <v>2</v>
       </c>
-      <c r="M82" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N82" s="19">
+      <c r="M82" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N82" s="18">
         <v>0.5</v>
       </c>
-      <c r="O82" s="19">
+      <c r="O82" s="18">
         <v>3.5</v>
       </c>
-      <c r="P82" s="19">
+      <c r="P82" s="18">
         <v>1.75</v>
       </c>
-      <c r="Q82" s="19"/>
-      <c r="R82" s="19"/>
+      <c r="Q82" s="18"/>
+      <c r="R82" s="18"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="11">
@@ -5209,26 +5230,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K83" s="19" t="s">
+      <c r="K83" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L83" s="19">
+      <c r="L83" s="18">
         <v>2</v>
       </c>
-      <c r="M83" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N83" s="19">
+      <c r="M83" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N83" s="18">
         <v>0.2</v>
       </c>
-      <c r="O83" s="19">
+      <c r="O83" s="18">
         <v>1.4</v>
       </c>
-      <c r="P83" s="19">
+      <c r="P83" s="18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="Q83" s="19"/>
-      <c r="R83" s="19"/>
+      <c r="Q83" s="18"/>
+      <c r="R83" s="18"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="11">
@@ -5251,26 +5272,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K84" s="19" t="s">
+      <c r="K84" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L84" s="19">
+      <c r="L84" s="18">
         <v>2</v>
       </c>
-      <c r="M84" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N84" s="19">
+      <c r="M84" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N84" s="18">
         <v>0.1</v>
       </c>
-      <c r="O84" s="19">
+      <c r="O84" s="18">
         <v>0.7</v>
       </c>
-      <c r="P84" s="19">
+      <c r="P84" s="18">
         <v>0.35000000000000003</v>
       </c>
-      <c r="Q84" s="19"/>
-      <c r="R84" s="19"/>
+      <c r="Q84" s="18"/>
+      <c r="R84" s="18"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="11">
@@ -5293,26 +5314,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K85" s="19" t="s">
+      <c r="K85" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L85" s="19">
+      <c r="L85" s="18">
         <v>2</v>
       </c>
-      <c r="M85" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N85" s="19">
+      <c r="M85" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N85" s="18">
         <v>0.05</v>
       </c>
-      <c r="O85" s="19">
+      <c r="O85" s="18">
         <v>0.35</v>
       </c>
-      <c r="P85" s="19">
+      <c r="P85" s="18">
         <v>0.17500000000000002</v>
       </c>
-      <c r="Q85" s="19"/>
-      <c r="R85" s="19"/>
+      <c r="Q85" s="18"/>
+      <c r="R85" s="18"/>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="11">
@@ -5335,26 +5356,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K86" s="19" t="s">
+      <c r="K86" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L86" s="19">
+      <c r="L86" s="18">
         <v>2</v>
       </c>
-      <c r="M86" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N86" s="19">
+      <c r="M86" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N86" s="18">
         <v>0.02</v>
       </c>
-      <c r="O86" s="19">
+      <c r="O86" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P86" s="19">
+      <c r="P86" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q86" s="19"/>
-      <c r="R86" s="19"/>
+      <c r="Q86" s="18"/>
+      <c r="R86" s="18"/>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="11">
@@ -5377,26 +5398,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K87" s="19" t="s">
+      <c r="K87" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L87" s="19">
+      <c r="L87" s="18">
         <v>2</v>
       </c>
-      <c r="M87" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N87" s="19">
+      <c r="M87" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N87" s="18">
         <v>0.01</v>
       </c>
-      <c r="O87" s="19">
+      <c r="O87" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P87" s="19">
+      <c r="P87" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q87" s="19"/>
-      <c r="R87" s="19"/>
+      <c r="Q87" s="18"/>
+      <c r="R87" s="18"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="11">
@@ -5419,26 +5440,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K88" s="19" t="s">
+      <c r="K88" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L88" s="19">
+      <c r="L88" s="18">
         <v>2</v>
       </c>
-      <c r="M88" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N88" s="19">
+      <c r="M88" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N88" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O88" s="19">
+      <c r="O88" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P88" s="19">
+      <c r="P88" s="18">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="Q88" s="19"/>
-      <c r="R88" s="19"/>
+      <c r="Q88" s="18"/>
+      <c r="R88" s="18"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="11">
@@ -5461,26 +5482,26 @@
         <f t="shared" si="5"/>
         <v>Not Done</v>
       </c>
-      <c r="K89" s="19" t="s">
+      <c r="K89" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L89" s="19">
+      <c r="L89" s="18">
         <v>2</v>
       </c>
-      <c r="M89" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N89" s="19">
+      <c r="M89" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N89" s="18">
         <v>2E-3</v>
       </c>
-      <c r="O89" s="19">
+      <c r="O89" s="18">
         <v>1.4E-2</v>
       </c>
-      <c r="P89" s="19">
+      <c r="P89" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="Q89" s="19"/>
-      <c r="R89" s="19"/>
+      <c r="Q89" s="18"/>
+      <c r="R89" s="18"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
@@ -5492,14 +5513,14 @@
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
-      <c r="K90" s="19"/>
-      <c r="L90" s="19"/>
-      <c r="M90" s="19"/>
-      <c r="N90" s="19"/>
-      <c r="O90" s="19"/>
-      <c r="P90" s="19"/>
-      <c r="Q90" s="19"/>
-      <c r="R90" s="19"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="18"/>
+      <c r="O90" s="18"/>
+      <c r="P90" s="18"/>
+      <c r="Q90" s="18"/>
+      <c r="R90" s="18"/>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
@@ -5522,26 +5543,26 @@
         <f t="shared" ref="G91:G101" si="6">IF(ISBLANK(D91),"Not Done",IF(AND(D91&lt;=E91,D91&gt;=C91),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="K91" s="19" t="s">
+      <c r="K91" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L91" s="19">
+      <c r="L91" s="18">
         <v>3</v>
       </c>
-      <c r="M91" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N91" s="19">
+      <c r="M91" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N91" s="18">
         <v>5</v>
       </c>
-      <c r="O91" s="19">
+      <c r="O91" s="18">
         <v>35</v>
       </c>
-      <c r="P91" s="19">
+      <c r="P91" s="18">
         <v>17.5</v>
       </c>
-      <c r="Q91" s="19"/>
-      <c r="R91" s="19"/>
+      <c r="Q91" s="18"/>
+      <c r="R91" s="18"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
@@ -5564,26 +5585,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K92" s="19" t="s">
+      <c r="K92" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L92" s="19">
+      <c r="L92" s="18">
         <v>3</v>
       </c>
-      <c r="M92" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N92" s="19">
+      <c r="M92" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N92" s="18">
         <v>2</v>
       </c>
-      <c r="O92" s="19">
+      <c r="O92" s="18">
         <v>14</v>
       </c>
-      <c r="P92" s="19">
+      <c r="P92" s="18">
         <v>7</v>
       </c>
-      <c r="Q92" s="19"/>
-      <c r="R92" s="19"/>
+      <c r="Q92" s="18"/>
+      <c r="R92" s="18"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
@@ -5606,26 +5627,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K93" s="19" t="s">
+      <c r="K93" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L93" s="19">
+      <c r="L93" s="18">
         <v>3</v>
       </c>
-      <c r="M93" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N93" s="19">
+      <c r="M93" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N93" s="18">
         <v>1</v>
       </c>
-      <c r="O93" s="19">
+      <c r="O93" s="18">
         <v>7</v>
       </c>
-      <c r="P93" s="19">
+      <c r="P93" s="18">
         <v>3.5</v>
       </c>
-      <c r="Q93" s="19"/>
-      <c r="R93" s="19"/>
+      <c r="Q93" s="18"/>
+      <c r="R93" s="18"/>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="11">
@@ -5648,26 +5669,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K94" s="19" t="s">
+      <c r="K94" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L94" s="19">
+      <c r="L94" s="18">
         <v>3</v>
       </c>
-      <c r="M94" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N94" s="19">
+      <c r="M94" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N94" s="18">
         <v>0.5</v>
       </c>
-      <c r="O94" s="19">
+      <c r="O94" s="18">
         <v>3.5</v>
       </c>
-      <c r="P94" s="19">
+      <c r="P94" s="18">
         <v>1.75</v>
       </c>
-      <c r="Q94" s="19"/>
-      <c r="R94" s="19"/>
+      <c r="Q94" s="18"/>
+      <c r="R94" s="18"/>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="11">
@@ -5690,26 +5711,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K95" s="19" t="s">
+      <c r="K95" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L95" s="19">
+      <c r="L95" s="18">
         <v>3</v>
       </c>
-      <c r="M95" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N95" s="19">
+      <c r="M95" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N95" s="18">
         <v>0.2</v>
       </c>
-      <c r="O95" s="19">
+      <c r="O95" s="18">
         <v>1.4</v>
       </c>
-      <c r="P95" s="19">
+      <c r="P95" s="18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="Q95" s="19"/>
-      <c r="R95" s="19"/>
+      <c r="Q95" s="18"/>
+      <c r="R95" s="18"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="11">
@@ -5732,26 +5753,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K96" s="19" t="s">
+      <c r="K96" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L96" s="19">
+      <c r="L96" s="18">
         <v>3</v>
       </c>
-      <c r="M96" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N96" s="19">
+      <c r="M96" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N96" s="18">
         <v>0.1</v>
       </c>
-      <c r="O96" s="19">
+      <c r="O96" s="18">
         <v>0.7</v>
       </c>
-      <c r="P96" s="19">
+      <c r="P96" s="18">
         <v>0.35000000000000003</v>
       </c>
-      <c r="Q96" s="19"/>
-      <c r="R96" s="19"/>
+      <c r="Q96" s="18"/>
+      <c r="R96" s="18"/>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="11">
@@ -5774,26 +5795,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K97" s="19" t="s">
+      <c r="K97" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L97" s="19">
+      <c r="L97" s="18">
         <v>3</v>
       </c>
-      <c r="M97" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N97" s="19">
+      <c r="M97" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N97" s="18">
         <v>0.05</v>
       </c>
-      <c r="O97" s="19">
+      <c r="O97" s="18">
         <v>0.35</v>
       </c>
-      <c r="P97" s="19">
+      <c r="P97" s="18">
         <v>0.17500000000000002</v>
       </c>
-      <c r="Q97" s="19"/>
-      <c r="R97" s="19"/>
+      <c r="Q97" s="18"/>
+      <c r="R97" s="18"/>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="11">
@@ -5816,26 +5837,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K98" s="19" t="s">
+      <c r="K98" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L98" s="19">
+      <c r="L98" s="18">
         <v>3</v>
       </c>
-      <c r="M98" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N98" s="19">
+      <c r="M98" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N98" s="18">
         <v>0.02</v>
       </c>
-      <c r="O98" s="19">
+      <c r="O98" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P98" s="19">
+      <c r="P98" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q98" s="19"/>
-      <c r="R98" s="19"/>
+      <c r="Q98" s="18"/>
+      <c r="R98" s="18"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="11">
@@ -5858,26 +5879,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K99" s="19" t="s">
+      <c r="K99" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L99" s="19">
+      <c r="L99" s="18">
         <v>3</v>
       </c>
-      <c r="M99" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N99" s="19">
+      <c r="M99" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N99" s="18">
         <v>0.01</v>
       </c>
-      <c r="O99" s="19">
+      <c r="O99" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P99" s="19">
+      <c r="P99" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q99" s="19"/>
-      <c r="R99" s="19"/>
+      <c r="Q99" s="18"/>
+      <c r="R99" s="18"/>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="11">
@@ -5900,26 +5921,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K100" s="19" t="s">
+      <c r="K100" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L100" s="19">
+      <c r="L100" s="18">
         <v>3</v>
       </c>
-      <c r="M100" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N100" s="19">
+      <c r="M100" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N100" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O100" s="19">
+      <c r="O100" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P100" s="19">
+      <c r="P100" s="18">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="Q100" s="19"/>
-      <c r="R100" s="19"/>
+      <c r="Q100" s="18"/>
+      <c r="R100" s="18"/>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="11">
@@ -5942,26 +5963,26 @@
         <f t="shared" si="6"/>
         <v>Not Done</v>
       </c>
-      <c r="K101" s="19" t="s">
+      <c r="K101" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L101" s="19">
+      <c r="L101" s="18">
         <v>3</v>
       </c>
-      <c r="M101" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N101" s="19">
+      <c r="M101" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N101" s="18">
         <v>2E-3</v>
       </c>
-      <c r="O101" s="19">
+      <c r="O101" s="18">
         <v>1.4E-2</v>
       </c>
-      <c r="P101" s="19">
+      <c r="P101" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="Q101" s="19"/>
-      <c r="R101" s="19"/>
+      <c r="Q101" s="18"/>
+      <c r="R101" s="18"/>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
@@ -5973,14 +5994,14 @@
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
-      <c r="K102" s="19"/>
-      <c r="L102" s="19"/>
-      <c r="M102" s="19"/>
-      <c r="N102" s="19"/>
-      <c r="O102" s="19"/>
-      <c r="P102" s="19"/>
-      <c r="Q102" s="19"/>
-      <c r="R102" s="19"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="18"/>
+      <c r="M102" s="18"/>
+      <c r="N102" s="18"/>
+      <c r="O102" s="18"/>
+      <c r="P102" s="18"/>
+      <c r="Q102" s="18"/>
+      <c r="R102" s="18"/>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
@@ -6003,26 +6024,26 @@
         <f t="shared" ref="G103:G113" si="7">IF(ISBLANK(D103),"Not Done",IF(AND(D103&lt;=E103,D103&gt;=C103),"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="K103" s="19" t="s">
+      <c r="K103" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L103" s="19">
+      <c r="L103" s="18">
         <v>4</v>
       </c>
-      <c r="M103" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N103" s="19">
+      <c r="M103" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N103" s="18">
         <v>5</v>
       </c>
-      <c r="O103" s="19">
+      <c r="O103" s="18">
         <v>35</v>
       </c>
-      <c r="P103" s="19">
+      <c r="P103" s="18">
         <v>17.5</v>
       </c>
-      <c r="Q103" s="19"/>
-      <c r="R103" s="19"/>
+      <c r="Q103" s="18"/>
+      <c r="R103" s="18"/>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="9">
@@ -6045,26 +6066,26 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K104" s="19" t="s">
+      <c r="K104" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L104" s="19">
+      <c r="L104" s="18">
         <v>4</v>
       </c>
-      <c r="M104" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N104" s="19">
+      <c r="M104" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N104" s="18">
         <v>2</v>
       </c>
-      <c r="O104" s="19">
+      <c r="O104" s="18">
         <v>14</v>
       </c>
-      <c r="P104" s="19">
+      <c r="P104" s="18">
         <v>7</v>
       </c>
-      <c r="Q104" s="19"/>
-      <c r="R104" s="19"/>
+      <c r="Q104" s="18"/>
+      <c r="R104" s="18"/>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="9">
@@ -6087,26 +6108,26 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K105" s="19" t="s">
+      <c r="K105" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L105" s="19">
+      <c r="L105" s="18">
         <v>4</v>
       </c>
-      <c r="M105" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N105" s="19">
+      <c r="M105" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N105" s="18">
         <v>1</v>
       </c>
-      <c r="O105" s="19">
+      <c r="O105" s="18">
         <v>7</v>
       </c>
-      <c r="P105" s="19">
+      <c r="P105" s="18">
         <v>3.5</v>
       </c>
-      <c r="Q105" s="19"/>
-      <c r="R105" s="19"/>
+      <c r="Q105" s="18"/>
+      <c r="R105" s="18"/>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="11">
@@ -6129,26 +6150,26 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K106" s="19" t="s">
+      <c r="K106" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L106" s="19">
+      <c r="L106" s="18">
         <v>4</v>
       </c>
-      <c r="M106" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N106" s="19">
+      <c r="M106" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N106" s="18">
         <v>0.5</v>
       </c>
-      <c r="O106" s="19">
+      <c r="O106" s="18">
         <v>3.5</v>
       </c>
-      <c r="P106" s="19">
+      <c r="P106" s="18">
         <v>1.75</v>
       </c>
-      <c r="Q106" s="19"/>
-      <c r="R106" s="19"/>
+      <c r="Q106" s="18"/>
+      <c r="R106" s="18"/>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="11">
@@ -6171,26 +6192,26 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K107" s="19" t="s">
+      <c r="K107" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L107" s="19">
+      <c r="L107" s="18">
         <v>4</v>
       </c>
-      <c r="M107" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N107" s="19">
+      <c r="M107" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N107" s="18">
         <v>0.2</v>
       </c>
-      <c r="O107" s="19">
+      <c r="O107" s="18">
         <v>1.4</v>
       </c>
-      <c r="P107" s="19">
+      <c r="P107" s="18">
         <v>0.70000000000000007</v>
       </c>
-      <c r="Q107" s="19"/>
-      <c r="R107" s="19"/>
+      <c r="Q107" s="18"/>
+      <c r="R107" s="18"/>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="11">
@@ -6213,26 +6234,26 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K108" s="19" t="s">
+      <c r="K108" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L108" s="19">
+      <c r="L108" s="18">
         <v>4</v>
       </c>
-      <c r="M108" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N108" s="19">
+      <c r="M108" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N108" s="18">
         <v>0.1</v>
       </c>
-      <c r="O108" s="19">
+      <c r="O108" s="18">
         <v>0.7</v>
       </c>
-      <c r="P108" s="19">
+      <c r="P108" s="18">
         <v>0.35000000000000003</v>
       </c>
-      <c r="Q108" s="19"/>
-      <c r="R108" s="19"/>
+      <c r="Q108" s="18"/>
+      <c r="R108" s="18"/>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="11">
@@ -6255,26 +6276,26 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K109" s="19" t="s">
+      <c r="K109" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L109" s="19">
+      <c r="L109" s="18">
         <v>4</v>
       </c>
-      <c r="M109" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N109" s="19">
+      <c r="M109" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N109" s="18">
         <v>0.05</v>
       </c>
-      <c r="O109" s="19">
+      <c r="O109" s="18">
         <v>0.35</v>
       </c>
-      <c r="P109" s="19">
+      <c r="P109" s="18">
         <v>0.17500000000000002</v>
       </c>
-      <c r="Q109" s="19"/>
-      <c r="R109" s="19"/>
+      <c r="Q109" s="18"/>
+      <c r="R109" s="18"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="11">
@@ -6297,26 +6318,26 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K110" s="19" t="s">
+      <c r="K110" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L110" s="19">
+      <c r="L110" s="18">
         <v>4</v>
       </c>
-      <c r="M110" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N110" s="19">
+      <c r="M110" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N110" s="18">
         <v>0.02</v>
       </c>
-      <c r="O110" s="19">
+      <c r="O110" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="P110" s="19">
+      <c r="P110" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q110" s="19"/>
-      <c r="R110" s="19"/>
+      <c r="Q110" s="18"/>
+      <c r="R110" s="18"/>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="11">
@@ -6339,26 +6360,26 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K111" s="19" t="s">
+      <c r="K111" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L111" s="19">
+      <c r="L111" s="18">
         <v>4</v>
       </c>
-      <c r="M111" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N111" s="19">
+      <c r="M111" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N111" s="18">
         <v>0.01</v>
       </c>
-      <c r="O111" s="19">
+      <c r="O111" s="18">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P111" s="19">
+      <c r="P111" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q111" s="19"/>
-      <c r="R111" s="19"/>
+      <c r="Q111" s="18"/>
+      <c r="R111" s="18"/>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="11">
@@ -6381,26 +6402,26 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K112" s="19" t="s">
+      <c r="K112" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L112" s="19">
+      <c r="L112" s="18">
         <v>4</v>
       </c>
-      <c r="M112" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N112" s="19">
+      <c r="M112" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N112" s="18">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="O112" s="19">
+      <c r="O112" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="P112" s="19">
+      <c r="P112" s="18">
         <v>1.7500000000000002E-2</v>
       </c>
-      <c r="Q112" s="19"/>
-      <c r="R112" s="19"/>
+      <c r="Q112" s="18"/>
+      <c r="R112" s="18"/>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="11">
@@ -6423,49 +6444,49 @@
         <f t="shared" si="7"/>
         <v>Not Done</v>
       </c>
-      <c r="K113" s="19" t="s">
+      <c r="K113" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="L113" s="19">
+      <c r="L113" s="18">
         <v>4</v>
       </c>
-      <c r="M113" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="N113" s="19">
+      <c r="M113" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N113" s="18">
         <v>2E-3</v>
       </c>
-      <c r="O113" s="19">
+      <c r="O113" s="18">
         <v>1.4E-2</v>
       </c>
-      <c r="P113" s="19">
+      <c r="P113" s="18">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="Q113" s="19"/>
-      <c r="R113" s="19"/>
+      <c r="Q113" s="18"/>
+      <c r="R113" s="18"/>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K114" s="19"/>
-      <c r="L114" s="19"/>
-      <c r="M114" s="19"/>
-      <c r="N114" s="19"/>
-      <c r="O114" s="19"/>
-      <c r="P114" s="19"/>
-      <c r="Q114" s="19"/>
-      <c r="R114" s="19"/>
+      <c r="K114" s="18"/>
+      <c r="L114" s="18"/>
+      <c r="M114" s="18"/>
+      <c r="N114" s="18"/>
+      <c r="O114" s="18"/>
+      <c r="P114" s="18"/>
+      <c r="Q114" s="18"/>
+      <c r="R114" s="18"/>
     </row>
     <row r="115" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K115" s="19"/>
-      <c r="L115" s="19"/>
-      <c r="M115" s="19"/>
-      <c r="N115" s="19"/>
-      <c r="O115" s="19"/>
-      <c r="P115" s="19"/>
-      <c r="Q115" s="19"/>
-      <c r="R115" s="19"/>
+      <c r="K115" s="18"/>
+      <c r="L115" s="18"/>
+      <c r="M115" s="18"/>
+      <c r="N115" s="18"/>
+      <c r="O115" s="18"/>
+      <c r="P115" s="18"/>
+      <c r="Q115" s="18"/>
+      <c r="R115" s="18"/>
     </row>
     <row r="116" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
@@ -6486,26 +6507,26 @@
       <c r="F116" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K116" s="19"/>
-      <c r="L116" s="19"/>
-      <c r="M116" s="19" t="s">
+      <c r="K116" s="18"/>
+      <c r="L116" s="18"/>
+      <c r="M116" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="N116" s="19"/>
-      <c r="O116" s="19"/>
-      <c r="P116" s="19"/>
-      <c r="Q116" s="19"/>
-      <c r="R116" s="19"/>
+      <c r="N116" s="18"/>
+      <c r="O116" s="18"/>
+      <c r="P116" s="18"/>
+      <c r="Q116" s="18"/>
+      <c r="R116" s="18"/>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="B117" s="10"/>
+      <c r="B117" s="19"/>
       <c r="C117" s="13">
         <v>350</v>
       </c>
-      <c r="D117" s="16" t="str">
+      <c r="D117" s="20" t="str">
         <f>IFERROR((350/B117),"Not Done")</f>
         <v>Not Done</v>
       </c>
@@ -6513,33 +6534,33 @@
         <v>55</v>
       </c>
       <c r="F117" s="10" t="str">
-        <f>IF(ISBLANK(B117),"Not Done",IF(B117&lt;=C117,"Pass","Fail"))</f>
-        <v>Not Done</v>
-      </c>
-      <c r="K117" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="L117" s="19">
+        <f>IF(ISBLANK(B117),"Not Done",IF(D117&gt;=C117,"Pass","Fail"))</f>
+        <v>Not Done</v>
+      </c>
+      <c r="K117" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="L117" s="18">
         <v>1</v>
       </c>
-      <c r="M117" s="19">
+      <c r="M117" s="18">
         <v>5</v>
       </c>
-      <c r="N117" s="19"/>
-      <c r="O117" s="19"/>
-      <c r="P117" s="19"/>
-      <c r="Q117" s="19"/>
-      <c r="R117" s="19"/>
+      <c r="N117" s="18"/>
+      <c r="O117" s="18"/>
+      <c r="P117" s="18"/>
+      <c r="Q117" s="18"/>
+      <c r="R117" s="18"/>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B118" s="10"/>
+      <c r="B118" s="19"/>
       <c r="C118" s="13">
         <v>350</v>
       </c>
-      <c r="D118" s="16" t="str">
+      <c r="D118" s="20" t="str">
         <f t="shared" ref="D118:D120" si="8">IFERROR((350/B118),"Not Done")</f>
         <v>Not Done</v>
       </c>
@@ -6547,33 +6568,33 @@
         <v>55</v>
       </c>
       <c r="F118" s="10" t="str">
-        <f t="shared" ref="F118:F120" si="9">IF(ISBLANK(B118),"Not Done",IF(B118&gt;=C118,"Pass","Fail"))</f>
-        <v>Not Done</v>
-      </c>
-      <c r="K118" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="L118" s="19">
+        <f t="shared" ref="F118:F120" si="9">IF(ISBLANK(B118),"Not Done",IF(D118&gt;=C118,"Pass","Fail"))</f>
+        <v>Not Done</v>
+      </c>
+      <c r="K118" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="L118" s="18">
         <v>2</v>
       </c>
-      <c r="M118" s="19">
+      <c r="M118" s="18">
         <v>5</v>
       </c>
-      <c r="N118" s="19"/>
-      <c r="O118" s="19"/>
-      <c r="P118" s="19"/>
-      <c r="Q118" s="19"/>
-      <c r="R118" s="19"/>
+      <c r="N118" s="18"/>
+      <c r="O118" s="18"/>
+      <c r="P118" s="18"/>
+      <c r="Q118" s="18"/>
+      <c r="R118" s="18"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B119" s="10"/>
+      <c r="B119" s="19"/>
       <c r="C119" s="13">
         <v>350</v>
       </c>
-      <c r="D119" s="16" t="str">
+      <c r="D119" s="20" t="str">
         <f t="shared" si="8"/>
         <v>Not Done</v>
       </c>
@@ -6584,30 +6605,30 @@
         <f t="shared" si="9"/>
         <v>Not Done</v>
       </c>
-      <c r="K119" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="L119" s="19">
+      <c r="K119" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="L119" s="18">
         <v>3</v>
       </c>
-      <c r="M119" s="19">
+      <c r="M119" s="18">
         <v>5</v>
       </c>
-      <c r="N119" s="19"/>
-      <c r="O119" s="19"/>
-      <c r="P119" s="19"/>
-      <c r="Q119" s="19"/>
-      <c r="R119" s="19"/>
+      <c r="N119" s="18"/>
+      <c r="O119" s="18"/>
+      <c r="P119" s="18"/>
+      <c r="Q119" s="18"/>
+      <c r="R119" s="18"/>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B120" s="10"/>
+      <c r="B120" s="19"/>
       <c r="C120" s="13">
         <v>350</v>
       </c>
-      <c r="D120" s="16" t="str">
+      <c r="D120" s="20" t="str">
         <f t="shared" si="8"/>
         <v>Not Done</v>
       </c>
@@ -6618,43 +6639,43 @@
         <f t="shared" si="9"/>
         <v>Not Done</v>
       </c>
-      <c r="K120" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="L120" s="19">
+      <c r="K120" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="L120" s="18">
         <v>4</v>
       </c>
-      <c r="M120" s="19">
+      <c r="M120" s="18">
         <v>5</v>
       </c>
-      <c r="N120" s="19"/>
-      <c r="O120" s="19"/>
-      <c r="P120" s="19"/>
-      <c r="Q120" s="19"/>
-      <c r="R120" s="19"/>
+      <c r="N120" s="18"/>
+      <c r="O120" s="18"/>
+      <c r="P120" s="18"/>
+      <c r="Q120" s="18"/>
+      <c r="R120" s="18"/>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K121" s="19"/>
-      <c r="L121" s="19"/>
-      <c r="M121" s="19"/>
-      <c r="N121" s="19"/>
-      <c r="O121" s="19"/>
-      <c r="P121" s="19"/>
-      <c r="Q121" s="19"/>
-      <c r="R121" s="19"/>
+      <c r="K121" s="18"/>
+      <c r="L121" s="18"/>
+      <c r="M121" s="18"/>
+      <c r="N121" s="18"/>
+      <c r="O121" s="18"/>
+      <c r="P121" s="18"/>
+      <c r="Q121" s="18"/>
+      <c r="R121" s="18"/>
     </row>
     <row r="122" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K122" s="19"/>
-      <c r="L122" s="19"/>
-      <c r="M122" s="19"/>
-      <c r="N122" s="19"/>
-      <c r="O122" s="19"/>
-      <c r="P122" s="19"/>
-      <c r="Q122" s="19"/>
-      <c r="R122" s="19"/>
+      <c r="K122" s="18"/>
+      <c r="L122" s="18"/>
+      <c r="M122" s="18"/>
+      <c r="N122" s="18"/>
+      <c r="O122" s="18"/>
+      <c r="P122" s="18"/>
+      <c r="Q122" s="18"/>
+      <c r="R122" s="18"/>
     </row>
     <row r="123" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
@@ -6672,14 +6693,14 @@
       <c r="E123" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K123" s="19" t="s">
+      <c r="K123" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="N123" s="19"/>
-      <c r="O123" s="19"/>
-      <c r="P123" s="19"/>
-      <c r="Q123" s="19"/>
-      <c r="R123" s="19"/>
+      <c r="N123" s="18"/>
+      <c r="O123" s="18"/>
+      <c r="P123" s="18"/>
+      <c r="Q123" s="18"/>
+      <c r="R123" s="18"/>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" s="10"/>
@@ -6695,74 +6716,74 @@
         <f>IF(ISBLANK(B124),"Not Done",IF(ABS(B124)&lt;=C124,"Pass","Fail"))</f>
         <v>Not Done</v>
       </c>
-      <c r="K124" s="19" t="s">
+      <c r="K124" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="M124" s="19">
+      <c r="M124" s="18">
         <v>10</v>
       </c>
-      <c r="N124" s="19"/>
-      <c r="O124" s="19"/>
-      <c r="P124" s="19"/>
-      <c r="Q124" s="19"/>
-      <c r="R124" s="19"/>
+      <c r="N124" s="18"/>
+      <c r="O124" s="18"/>
+      <c r="P124" s="18"/>
+      <c r="Q124" s="18"/>
+      <c r="R124" s="18"/>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K125" s="19"/>
-      <c r="L125" s="19"/>
-      <c r="M125" s="19"/>
-      <c r="N125" s="19"/>
-      <c r="O125" s="19"/>
-      <c r="P125" s="19"/>
-      <c r="Q125" s="19"/>
-      <c r="R125" s="19"/>
+      <c r="K125" s="18"/>
+      <c r="L125" s="18"/>
+      <c r="M125" s="18"/>
+      <c r="N125" s="18"/>
+      <c r="O125" s="18"/>
+      <c r="P125" s="18"/>
+      <c r="Q125" s="18"/>
+      <c r="R125" s="18"/>
     </row>
     <row r="126" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K126" s="19"/>
-      <c r="L126" s="19"/>
-      <c r="M126" s="19"/>
-      <c r="N126" s="19"/>
-      <c r="O126" s="19"/>
-      <c r="P126" s="19"/>
-      <c r="Q126" s="19"/>
-      <c r="R126" s="19"/>
+      <c r="K126" s="18"/>
+      <c r="L126" s="18"/>
+      <c r="M126" s="18"/>
+      <c r="N126" s="18"/>
+      <c r="O126" s="18"/>
+      <c r="P126" s="18"/>
+      <c r="Q126" s="18"/>
+      <c r="R126" s="18"/>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B127" s="18" t="s">
-        <v>72</v>
+      <c r="B127" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K127" s="19" t="s">
+      <c r="K127" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="L127" s="19" t="s">
+      <c r="L127" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="M127" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="N127" s="19" t="s">
+      <c r="M127" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="O127" s="19" t="s">
+      <c r="N127" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="P127" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q127" s="19" t="s">
+      <c r="O127" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="R127" s="19" t="s">
-        <v>71</v>
+      <c r="P127" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q127" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="R127" s="18" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
@@ -6771,16 +6792,16 @@
       </c>
       <c r="B128" s="7"/>
       <c r="C128" s="8"/>
-      <c r="K128" s="19"/>
-      <c r="L128" s="19"/>
-      <c r="M128" s="19"/>
-      <c r="N128" s="19"/>
-      <c r="O128" s="19"/>
-      <c r="P128" s="19"/>
-      <c r="Q128" s="19"/>
-      <c r="R128" s="19"/>
-    </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K128" s="18"/>
+      <c r="L128" s="18"/>
+      <c r="M128" s="18"/>
+      <c r="N128" s="18"/>
+      <c r="O128" s="18"/>
+      <c r="P128" s="18"/>
+      <c r="Q128" s="18"/>
+      <c r="R128" s="18"/>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="10" t="s">
         <v>29</v>
       </c>
@@ -6789,31 +6810,27 @@
         <f>IF(ISBLANK(B129),"Not Done",B129)</f>
         <v>Not Done</v>
       </c>
-      <c r="K129" s="19" t="s">
+      <c r="K129" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="L129" s="19">
+      <c r="L129" s="18">
         <v>1</v>
       </c>
-      <c r="M129" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="N129" s="19">
+      <c r="M129" s="18">
         <v>0.1</v>
       </c>
-      <c r="O129" s="19">
+      <c r="N129" s="18">
         <v>0.05</v>
       </c>
-      <c r="P129" s="19"/>
-      <c r="Q129" s="19">
+      <c r="O129" s="18">
         <v>50</v>
       </c>
-      <c r="R129" s="19">
+      <c r="P129" s="18">
         <v>350</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A130" s="17" t="s">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A130" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B130" s="10"/>
@@ -6821,30 +6838,26 @@
         <f t="shared" ref="C130:C134" si="10">IF(ISBLANK(B130),"Not Done",B130)</f>
         <v>Not Done</v>
       </c>
-      <c r="K130" s="19" t="s">
+      <c r="K130" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="L130" s="19">
+      <c r="L130" s="18">
         <v>2</v>
       </c>
-      <c r="M130" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="N130" s="19">
+      <c r="M130" s="18">
         <v>0.1</v>
       </c>
-      <c r="O130" s="19">
+      <c r="N130" s="18">
         <v>0.05</v>
       </c>
-      <c r="P130" s="19"/>
-      <c r="Q130" s="19">
+      <c r="O130" s="18">
         <v>50</v>
       </c>
-      <c r="R130" s="19">
+      <c r="P130" s="18">
         <v>350</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="10" t="s">
         <v>33</v>
       </c>
@@ -6853,31 +6866,27 @@
         <f t="shared" si="10"/>
         <v>Not Done</v>
       </c>
-      <c r="K131" s="19" t="s">
+      <c r="K131" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="L131" s="19">
+      <c r="L131" s="18">
         <v>3</v>
       </c>
-      <c r="M131" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="N131" s="19">
+      <c r="M131" s="18">
         <v>0.1</v>
       </c>
-      <c r="O131" s="19">
+      <c r="N131" s="18">
         <v>0.05</v>
       </c>
-      <c r="P131" s="19"/>
-      <c r="Q131" s="19">
+      <c r="O131" s="18">
         <v>50</v>
       </c>
-      <c r="R131" s="19">
+      <c r="P131" s="18">
         <v>350</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A132" s="17" t="s">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A132" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B132" s="10"/>
@@ -6885,71 +6894,62 @@
         <f t="shared" si="10"/>
         <v>Not Done</v>
       </c>
-      <c r="K132" s="19" t="s">
+      <c r="K132" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="L132" s="19">
+      <c r="L132" s="18">
         <v>4</v>
       </c>
-      <c r="M132" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="N132" s="19">
+      <c r="M132" s="18">
         <v>0.1</v>
       </c>
-      <c r="O132" s="19">
+      <c r="N132" s="18">
         <v>0.05</v>
       </c>
-      <c r="P132" s="19"/>
-      <c r="Q132" s="19">
+      <c r="O132" s="18">
         <v>50</v>
       </c>
-      <c r="R132" s="19">
+      <c r="P132" s="18">
         <v>350</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B133" s="7"/>
       <c r="C133" s="8"/>
-      <c r="K133" s="19"/>
-      <c r="L133" s="19"/>
-      <c r="M133" s="19"/>
-      <c r="N133" s="19"/>
-      <c r="O133" s="19"/>
-      <c r="P133" s="19"/>
-      <c r="Q133" s="19"/>
-      <c r="R133" s="19"/>
-    </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K133" s="18"/>
+      <c r="L133" s="18"/>
+      <c r="M133" s="18"/>
+      <c r="N133" s="18"/>
+      <c r="O133" s="18"/>
+      <c r="P133" s="18"/>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B134" s="10"/>
       <c r="C134" s="10" t="str">
         <f t="shared" si="10"/>
         <v>Not Done</v>
       </c>
-      <c r="K134" s="19" t="s">
+      <c r="K134" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="L134" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="M134" s="19"/>
-      <c r="N134" s="19"/>
-      <c r="O134" s="19">
+      <c r="L134" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="N134" s="18">
         <v>0.2</v>
       </c>
-      <c r="P134" s="19"/>
-      <c r="Q134" s="19"/>
-      <c r="R134" s="19">
+      <c r="O134" s="18"/>
+      <c r="P134" s="18">
         <v>200</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C136" s="14" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
add model name to test sheet
</commit_message>
<xml_diff>
--- a/testsheets/666_Keysight_DSOX3034A.xlsx
+++ b/testsheets/666_Keysight_DSOX3034A.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Software\Python\oscilloscope\testsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C244BE56-5784-45A9-8F98-74F8C6A99003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE7BD0E-D4B2-4B6B-8908-B469CF9380B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="Model">Sheet!$B$6</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet!$A$1:$G$136</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet!$1:$12</definedName>
     <definedName name="StartCell">Sheet!$K$16</definedName>
@@ -479,7 +480,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="284">
+  <dxfs count="41">
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -489,6 +490,93 @@
       <font>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF00B050"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -522,14 +610,11 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -539,14 +624,25 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFE699"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -573,1482 +669,13 @@
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
@@ -2061,7 +688,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF99FF"/>
+          <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2069,13 +696,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF99FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFE699"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2403,8 +1023,8 @@
   </sheetPr>
   <dimension ref="A3:S136"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6956,1236 +5576,185 @@
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="B5 B129:B132">
-    <cfRule type="containsText" dxfId="283" priority="13" operator="containsText" text="highlight">
+  <conditionalFormatting sqref="A124:B124">
+    <cfRule type="containsText" dxfId="40" priority="295" operator="containsText" text="highlight">
+      <formula>ISBLANK(A124)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5 B129:C132">
+    <cfRule type="containsText" dxfId="39" priority="13" operator="containsText" text="highlight">
       <formula>ISBLANK(B5)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="containsText" dxfId="38" priority="15" operator="containsText" text="highlight">
+      <formula>ISBLANK(B7)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="containsText" dxfId="37" priority="17" operator="containsText" text="highlight">
+      <formula>ISBLANK(B11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B117:B120">
+    <cfRule type="containsText" dxfId="36" priority="4" operator="containsText" text="highlight">
+      <formula>ISBLANK(B117)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B134:C134">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="highlight">
+      <formula>ISBLANK(B134)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C129:C132">
+    <cfRule type="containsText" dxfId="34" priority="305" operator="containsText" text="highlight">
+      <formula>C129="Pass"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="304" operator="containsText" text="highlight">
+      <formula>C129="Fail"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C134">
+    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="highlight">
+      <formula>C134="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="highlight">
+      <formula>C134="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:D26">
+    <cfRule type="containsText" dxfId="30" priority="19" operator="containsText" text="highlight">
+      <formula>ISBLANK(D16)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:D38">
+    <cfRule type="containsText" dxfId="29" priority="52" operator="containsText" text="highlight">
+      <formula>ISBLANK(D28)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:D50">
+    <cfRule type="containsText" dxfId="28" priority="85" operator="containsText" text="highlight">
+      <formula>ISBLANK(D40)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52:D62">
+    <cfRule type="containsText" dxfId="27" priority="118" operator="containsText" text="highlight">
+      <formula>ISBLANK(D52)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67:D77">
+    <cfRule type="containsText" dxfId="26" priority="151" operator="containsText" text="highlight">
+      <formula>ISBLANK(D67)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D79:D89">
+    <cfRule type="containsText" dxfId="25" priority="184" operator="containsText" text="highlight">
+      <formula>ISBLANK(D79)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D91:D101">
+    <cfRule type="containsText" dxfId="24" priority="217" operator="containsText" text="highlight">
+      <formula>ISBLANK(D91)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D103:D113">
+    <cfRule type="containsText" dxfId="23" priority="250" operator="containsText" text="highlight">
+      <formula>ISBLANK(D103)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E124">
+    <cfRule type="containsText" dxfId="22" priority="297" operator="containsText" text="highlight">
+      <formula>E124="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="298" operator="containsText" text="highlight">
+      <formula>E124="Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="282" priority="14" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="20" priority="14" operator="containsText" text="highlight">
       <formula>ISBLANK(F5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="containsText" dxfId="281" priority="15" operator="containsText" text="highlight">
-      <formula>ISBLANK(B7)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="containsText" dxfId="280" priority="16" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="highlight">
       <formula>ISBLANK(F9)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="279" priority="17" operator="containsText" text="highlight">
-      <formula>ISBLANK(B11)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="containsText" dxfId="278" priority="18" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="highlight">
       <formula>ISBLANK(F10)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="containsText" dxfId="277" priority="19" operator="containsText" text="highlight">
-      <formula>ISBLANK(D16)</formula>
+  <conditionalFormatting sqref="F117:F120">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="highlight">
+      <formula>F117="Fail"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="highlight">
+      <formula>F117="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16">
-    <cfRule type="containsText" dxfId="276" priority="20" operator="containsText" text="highlight">
+  <conditionalFormatting sqref="G16:G26">
+    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="highlight">
       <formula>G16="Fail"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="275" priority="21" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="14" priority="21" operator="containsText" text="highlight">
       <formula>G16="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="containsText" dxfId="274" priority="22" operator="containsText" text="highlight">
-      <formula>ISBLANK(D17)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G17">
-    <cfRule type="containsText" dxfId="273" priority="23" operator="containsText" text="highlight">
-      <formula>G17="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="272" priority="24" operator="containsText" text="highlight">
-      <formula>G17="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="containsText" dxfId="271" priority="25" operator="containsText" text="highlight">
-      <formula>ISBLANK(D18)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18">
-    <cfRule type="containsText" dxfId="270" priority="26" operator="containsText" text="highlight">
-      <formula>G18="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="269" priority="27" operator="containsText" text="highlight">
-      <formula>G18="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="containsText" dxfId="268" priority="28" operator="containsText" text="highlight">
-      <formula>ISBLANK(D19)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G19">
-    <cfRule type="containsText" dxfId="267" priority="29" operator="containsText" text="highlight">
-      <formula>G19="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="266" priority="30" operator="containsText" text="highlight">
-      <formula>G19="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D20">
-    <cfRule type="containsText" dxfId="265" priority="31" operator="containsText" text="highlight">
-      <formula>ISBLANK(D20)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
-    <cfRule type="containsText" dxfId="264" priority="32" operator="containsText" text="highlight">
-      <formula>G20="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="263" priority="33" operator="containsText" text="highlight">
-      <formula>G20="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
-    <cfRule type="containsText" dxfId="262" priority="34" operator="containsText" text="highlight">
-      <formula>ISBLANK(D21)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G21">
-    <cfRule type="containsText" dxfId="261" priority="35" operator="containsText" text="highlight">
-      <formula>G21="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="260" priority="36" operator="containsText" text="highlight">
-      <formula>G21="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="containsText" dxfId="259" priority="37" operator="containsText" text="highlight">
-      <formula>ISBLANK(D22)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G22">
-    <cfRule type="containsText" dxfId="258" priority="38" operator="containsText" text="highlight">
-      <formula>G22="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="257" priority="39" operator="containsText" text="highlight">
-      <formula>G22="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
-    <cfRule type="containsText" dxfId="256" priority="40" operator="containsText" text="highlight">
-      <formula>ISBLANK(D23)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G23">
-    <cfRule type="containsText" dxfId="255" priority="41" operator="containsText" text="highlight">
-      <formula>G23="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="254" priority="42" operator="containsText" text="highlight">
-      <formula>G23="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
-    <cfRule type="containsText" dxfId="253" priority="43" operator="containsText" text="highlight">
-      <formula>ISBLANK(D24)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G24">
-    <cfRule type="containsText" dxfId="252" priority="44" operator="containsText" text="highlight">
-      <formula>G24="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="251" priority="45" operator="containsText" text="highlight">
-      <formula>G24="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
-    <cfRule type="containsText" dxfId="250" priority="46" operator="containsText" text="highlight">
-      <formula>ISBLANK(D25)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G25">
-    <cfRule type="containsText" dxfId="249" priority="47" operator="containsText" text="highlight">
-      <formula>G25="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="248" priority="48" operator="containsText" text="highlight">
-      <formula>G25="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
-    <cfRule type="containsText" dxfId="247" priority="49" operator="containsText" text="highlight">
-      <formula>ISBLANK(D26)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G26">
-    <cfRule type="containsText" dxfId="246" priority="50" operator="containsText" text="highlight">
-      <formula>G26="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="245" priority="51" operator="containsText" text="highlight">
-      <formula>G26="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
-    <cfRule type="containsText" dxfId="244" priority="52" operator="containsText" text="highlight">
-      <formula>ISBLANK(D28)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="containsText" dxfId="243" priority="53" operator="containsText" text="highlight">
+  <conditionalFormatting sqref="G28:G38">
+    <cfRule type="containsText" dxfId="13" priority="53" operator="containsText" text="highlight">
       <formula>G28="Fail"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="54" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="12" priority="54" operator="containsText" text="highlight">
       <formula>G28="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D29">
-    <cfRule type="containsText" dxfId="241" priority="55" operator="containsText" text="highlight">
-      <formula>ISBLANK(D29)</formula>
+  <conditionalFormatting sqref="G40:G50">
+    <cfRule type="containsText" dxfId="11" priority="87" operator="containsText" text="highlight">
+      <formula>G40="Pass"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="86" operator="containsText" text="highlight">
+      <formula>G40="Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G29">
-    <cfRule type="containsText" dxfId="240" priority="56" operator="containsText" text="highlight">
-      <formula>G29="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="239" priority="57" operator="containsText" text="highlight">
-      <formula>G29="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
-    <cfRule type="containsText" dxfId="238" priority="58" operator="containsText" text="highlight">
-      <formula>ISBLANK(D30)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G30">
-    <cfRule type="containsText" dxfId="237" priority="59" operator="containsText" text="highlight">
-      <formula>G30="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="236" priority="60" operator="containsText" text="highlight">
-      <formula>G30="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
-    <cfRule type="containsText" dxfId="235" priority="61" operator="containsText" text="highlight">
-      <formula>ISBLANK(D31)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G31">
-    <cfRule type="containsText" dxfId="234" priority="62" operator="containsText" text="highlight">
-      <formula>G31="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="233" priority="63" operator="containsText" text="highlight">
-      <formula>G31="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
-    <cfRule type="containsText" dxfId="232" priority="64" operator="containsText" text="highlight">
-      <formula>ISBLANK(D32)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G32">
-    <cfRule type="containsText" dxfId="231" priority="65" operator="containsText" text="highlight">
-      <formula>G32="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="66" operator="containsText" text="highlight">
-      <formula>G32="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
-    <cfRule type="containsText" dxfId="229" priority="67" operator="containsText" text="highlight">
-      <formula>ISBLANK(D33)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G33">
-    <cfRule type="containsText" dxfId="228" priority="68" operator="containsText" text="highlight">
-      <formula>G33="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="227" priority="69" operator="containsText" text="highlight">
-      <formula>G33="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
-    <cfRule type="containsText" dxfId="226" priority="70" operator="containsText" text="highlight">
-      <formula>ISBLANK(D34)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G34">
-    <cfRule type="containsText" dxfId="225" priority="71" operator="containsText" text="highlight">
-      <formula>G34="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="224" priority="72" operator="containsText" text="highlight">
-      <formula>G34="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="containsText" dxfId="223" priority="73" operator="containsText" text="highlight">
-      <formula>ISBLANK(D35)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G35">
-    <cfRule type="containsText" dxfId="222" priority="74" operator="containsText" text="highlight">
-      <formula>G35="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="221" priority="75" operator="containsText" text="highlight">
-      <formula>G35="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="containsText" dxfId="220" priority="76" operator="containsText" text="highlight">
-      <formula>ISBLANK(D36)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G36">
-    <cfRule type="containsText" dxfId="219" priority="77" operator="containsText" text="highlight">
-      <formula>G36="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="78" operator="containsText" text="highlight">
-      <formula>G36="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="containsText" dxfId="217" priority="79" operator="containsText" text="highlight">
-      <formula>ISBLANK(D37)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G37">
-    <cfRule type="containsText" dxfId="216" priority="80" operator="containsText" text="highlight">
-      <formula>G37="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="215" priority="81" operator="containsText" text="highlight">
-      <formula>G37="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
-    <cfRule type="containsText" dxfId="214" priority="82" operator="containsText" text="highlight">
-      <formula>ISBLANK(D38)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G38">
-    <cfRule type="containsText" dxfId="213" priority="83" operator="containsText" text="highlight">
-      <formula>G38="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="212" priority="84" operator="containsText" text="highlight">
-      <formula>G38="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="containsText" dxfId="211" priority="85" operator="containsText" text="highlight">
-      <formula>ISBLANK(D40)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G40">
-    <cfRule type="containsText" dxfId="210" priority="86" operator="containsText" text="highlight">
-      <formula>G40="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="209" priority="87" operator="containsText" text="highlight">
-      <formula>G40="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="containsText" dxfId="208" priority="88" operator="containsText" text="highlight">
-      <formula>ISBLANK(D41)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G41">
-    <cfRule type="containsText" dxfId="207" priority="89" operator="containsText" text="highlight">
-      <formula>G41="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="90" operator="containsText" text="highlight">
-      <formula>G41="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D42">
-    <cfRule type="containsText" dxfId="205" priority="91" operator="containsText" text="highlight">
-      <formula>ISBLANK(D42)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G42">
-    <cfRule type="containsText" dxfId="204" priority="92" operator="containsText" text="highlight">
-      <formula>G42="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="203" priority="93" operator="containsText" text="highlight">
-      <formula>G42="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
-    <cfRule type="containsText" dxfId="202" priority="94" operator="containsText" text="highlight">
-      <formula>ISBLANK(D43)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G43">
-    <cfRule type="containsText" dxfId="201" priority="95" operator="containsText" text="highlight">
-      <formula>G43="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="200" priority="96" operator="containsText" text="highlight">
-      <formula>G43="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="containsText" dxfId="199" priority="97" operator="containsText" text="highlight">
-      <formula>ISBLANK(D44)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G44">
-    <cfRule type="containsText" dxfId="198" priority="98" operator="containsText" text="highlight">
-      <formula>G44="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="197" priority="99" operator="containsText" text="highlight">
-      <formula>G44="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="containsText" dxfId="196" priority="100" operator="containsText" text="highlight">
-      <formula>ISBLANK(D45)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="195" priority="101" operator="containsText" text="highlight">
-      <formula>G45="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="102" operator="containsText" text="highlight">
-      <formula>G45="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46">
-    <cfRule type="containsText" dxfId="193" priority="103" operator="containsText" text="highlight">
-      <formula>ISBLANK(D46)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G46">
-    <cfRule type="containsText" dxfId="192" priority="104" operator="containsText" text="highlight">
-      <formula>G46="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="105" operator="containsText" text="highlight">
-      <formula>G46="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="containsText" dxfId="190" priority="106" operator="containsText" text="highlight">
-      <formula>ISBLANK(D47)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G47">
-    <cfRule type="containsText" dxfId="189" priority="107" operator="containsText" text="highlight">
-      <formula>G47="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="188" priority="108" operator="containsText" text="highlight">
-      <formula>G47="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
-    <cfRule type="containsText" dxfId="187" priority="109" operator="containsText" text="highlight">
-      <formula>ISBLANK(D48)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G48">
-    <cfRule type="containsText" dxfId="186" priority="110" operator="containsText" text="highlight">
-      <formula>G48="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="111" operator="containsText" text="highlight">
-      <formula>G48="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
-    <cfRule type="containsText" dxfId="184" priority="112" operator="containsText" text="highlight">
-      <formula>ISBLANK(D49)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G49">
-    <cfRule type="containsText" dxfId="183" priority="113" operator="containsText" text="highlight">
-      <formula>G49="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="182" priority="114" operator="containsText" text="highlight">
-      <formula>G49="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D50">
-    <cfRule type="containsText" dxfId="181" priority="115" operator="containsText" text="highlight">
-      <formula>ISBLANK(D50)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G50">
-    <cfRule type="containsText" dxfId="180" priority="116" operator="containsText" text="highlight">
-      <formula>G50="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="117" operator="containsText" text="highlight">
-      <formula>G50="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
-    <cfRule type="containsText" dxfId="178" priority="118" operator="containsText" text="highlight">
-      <formula>ISBLANK(D52)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G52">
-    <cfRule type="containsText" dxfId="177" priority="119" operator="containsText" text="highlight">
+  <conditionalFormatting sqref="G52:G62">
+    <cfRule type="containsText" dxfId="9" priority="119" operator="containsText" text="highlight">
       <formula>G52="Fail"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="120" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="8" priority="120" operator="containsText" text="highlight">
       <formula>G52="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D53">
-    <cfRule type="containsText" dxfId="175" priority="121" operator="containsText" text="highlight">
-      <formula>ISBLANK(D53)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G53">
-    <cfRule type="containsText" dxfId="174" priority="122" operator="containsText" text="highlight">
-      <formula>G53="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="173" priority="123" operator="containsText" text="highlight">
-      <formula>G53="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="containsText" dxfId="172" priority="124" operator="containsText" text="highlight">
-      <formula>ISBLANK(D54)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G54">
-    <cfRule type="containsText" dxfId="171" priority="125" operator="containsText" text="highlight">
-      <formula>G54="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="170" priority="126" operator="containsText" text="highlight">
-      <formula>G54="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
-    <cfRule type="containsText" dxfId="169" priority="127" operator="containsText" text="highlight">
-      <formula>ISBLANK(D55)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G55">
-    <cfRule type="containsText" dxfId="168" priority="128" operator="containsText" text="highlight">
-      <formula>G55="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="129" operator="containsText" text="highlight">
-      <formula>G55="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
-    <cfRule type="containsText" dxfId="166" priority="130" operator="containsText" text="highlight">
-      <formula>ISBLANK(D56)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G56">
-    <cfRule type="containsText" dxfId="165" priority="131" operator="containsText" text="highlight">
-      <formula>G56="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="164" priority="132" operator="containsText" text="highlight">
-      <formula>G56="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="containsText" dxfId="163" priority="133" operator="containsText" text="highlight">
-      <formula>ISBLANK(D57)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G57">
-    <cfRule type="containsText" dxfId="162" priority="134" operator="containsText" text="highlight">
-      <formula>G57="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="161" priority="135" operator="containsText" text="highlight">
-      <formula>G57="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="containsText" dxfId="160" priority="136" operator="containsText" text="highlight">
-      <formula>ISBLANK(D58)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G58">
-    <cfRule type="containsText" dxfId="159" priority="137" operator="containsText" text="highlight">
-      <formula>G58="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="158" priority="138" operator="containsText" text="highlight">
-      <formula>G58="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
-    <cfRule type="containsText" dxfId="157" priority="139" operator="containsText" text="highlight">
-      <formula>ISBLANK(D59)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G59">
-    <cfRule type="containsText" dxfId="156" priority="140" operator="containsText" text="highlight">
-      <formula>G59="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="155" priority="141" operator="containsText" text="highlight">
-      <formula>G59="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="containsText" dxfId="154" priority="142" operator="containsText" text="highlight">
-      <formula>ISBLANK(D60)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G60">
-    <cfRule type="containsText" dxfId="153" priority="143" operator="containsText" text="highlight">
-      <formula>G60="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="144" operator="containsText" text="highlight">
-      <formula>G60="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="containsText" dxfId="151" priority="145" operator="containsText" text="highlight">
-      <formula>ISBLANK(D61)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G61">
-    <cfRule type="containsText" dxfId="150" priority="146" operator="containsText" text="highlight">
-      <formula>G61="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="149" priority="147" operator="containsText" text="highlight">
-      <formula>G61="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="containsText" dxfId="148" priority="148" operator="containsText" text="highlight">
-      <formula>ISBLANK(D62)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G62">
-    <cfRule type="containsText" dxfId="147" priority="149" operator="containsText" text="highlight">
-      <formula>G62="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="150" operator="containsText" text="highlight">
-      <formula>G62="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67">
-    <cfRule type="containsText" dxfId="145" priority="151" operator="containsText" text="highlight">
-      <formula>ISBLANK(D67)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G67">
-    <cfRule type="containsText" dxfId="144" priority="152" operator="containsText" text="highlight">
+  <conditionalFormatting sqref="G67:G77">
+    <cfRule type="containsText" dxfId="7" priority="152" operator="containsText" text="highlight">
       <formula>G67="Fail"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="153" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="6" priority="153" operator="containsText" text="highlight">
       <formula>G67="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D68">
-    <cfRule type="containsText" dxfId="142" priority="154" operator="containsText" text="highlight">
-      <formula>ISBLANK(D68)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G68">
-    <cfRule type="containsText" dxfId="141" priority="155" operator="containsText" text="highlight">
-      <formula>G68="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="156" operator="containsText" text="highlight">
-      <formula>G68="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D69">
-    <cfRule type="containsText" dxfId="139" priority="157" operator="containsText" text="highlight">
-      <formula>ISBLANK(D69)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G69">
-    <cfRule type="containsText" dxfId="138" priority="158" operator="containsText" text="highlight">
-      <formula>G69="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="159" operator="containsText" text="highlight">
-      <formula>G69="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D70">
-    <cfRule type="containsText" dxfId="136" priority="160" operator="containsText" text="highlight">
-      <formula>ISBLANK(D70)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G70">
-    <cfRule type="containsText" dxfId="135" priority="161" operator="containsText" text="highlight">
-      <formula>G70="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="162" operator="containsText" text="highlight">
-      <formula>G70="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D71">
-    <cfRule type="containsText" dxfId="133" priority="163" operator="containsText" text="highlight">
-      <formula>ISBLANK(D71)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G71">
-    <cfRule type="containsText" dxfId="132" priority="164" operator="containsText" text="highlight">
-      <formula>G71="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="165" operator="containsText" text="highlight">
-      <formula>G71="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D72">
-    <cfRule type="containsText" dxfId="130" priority="166" operator="containsText" text="highlight">
-      <formula>ISBLANK(D72)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G72">
-    <cfRule type="containsText" dxfId="129" priority="167" operator="containsText" text="highlight">
-      <formula>G72="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="168" operator="containsText" text="highlight">
-      <formula>G72="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D73">
-    <cfRule type="containsText" dxfId="127" priority="169" operator="containsText" text="highlight">
-      <formula>ISBLANK(D73)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G73">
-    <cfRule type="containsText" dxfId="126" priority="170" operator="containsText" text="highlight">
-      <formula>G73="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="171" operator="containsText" text="highlight">
-      <formula>G73="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D74">
-    <cfRule type="containsText" dxfId="124" priority="172" operator="containsText" text="highlight">
-      <formula>ISBLANK(D74)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G74">
-    <cfRule type="containsText" dxfId="123" priority="173" operator="containsText" text="highlight">
-      <formula>G74="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="174" operator="containsText" text="highlight">
-      <formula>G74="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D75">
-    <cfRule type="containsText" dxfId="121" priority="175" operator="containsText" text="highlight">
-      <formula>ISBLANK(D75)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G75">
-    <cfRule type="containsText" dxfId="120" priority="176" operator="containsText" text="highlight">
-      <formula>G75="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="177" operator="containsText" text="highlight">
-      <formula>G75="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D76">
-    <cfRule type="containsText" dxfId="118" priority="178" operator="containsText" text="highlight">
-      <formula>ISBLANK(D76)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G76">
-    <cfRule type="containsText" dxfId="117" priority="179" operator="containsText" text="highlight">
-      <formula>G76="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="180" operator="containsText" text="highlight">
-      <formula>G76="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D77">
-    <cfRule type="containsText" dxfId="115" priority="181" operator="containsText" text="highlight">
-      <formula>ISBLANK(D77)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G77">
-    <cfRule type="containsText" dxfId="114" priority="182" operator="containsText" text="highlight">
-      <formula>G77="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="183" operator="containsText" text="highlight">
-      <formula>G77="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D79">
-    <cfRule type="containsText" dxfId="112" priority="184" operator="containsText" text="highlight">
-      <formula>ISBLANK(D79)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G79">
-    <cfRule type="containsText" dxfId="111" priority="185" operator="containsText" text="highlight">
+  <conditionalFormatting sqref="G79:G89">
+    <cfRule type="containsText" dxfId="5" priority="185" operator="containsText" text="highlight">
       <formula>G79="Fail"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="186" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="4" priority="186" operator="containsText" text="highlight">
       <formula>G79="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D80">
-    <cfRule type="containsText" dxfId="109" priority="187" operator="containsText" text="highlight">
-      <formula>ISBLANK(D80)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G80">
-    <cfRule type="containsText" dxfId="108" priority="188" operator="containsText" text="highlight">
-      <formula>G80="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="189" operator="containsText" text="highlight">
-      <formula>G80="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D81">
-    <cfRule type="containsText" dxfId="106" priority="190" operator="containsText" text="highlight">
-      <formula>ISBLANK(D81)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G81">
-    <cfRule type="containsText" dxfId="105" priority="191" operator="containsText" text="highlight">
-      <formula>G81="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="192" operator="containsText" text="highlight">
-      <formula>G81="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D82">
-    <cfRule type="containsText" dxfId="103" priority="193" operator="containsText" text="highlight">
-      <formula>ISBLANK(D82)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G82">
-    <cfRule type="containsText" dxfId="102" priority="194" operator="containsText" text="highlight">
-      <formula>G82="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="195" operator="containsText" text="highlight">
-      <formula>G82="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D83">
-    <cfRule type="containsText" dxfId="100" priority="196" operator="containsText" text="highlight">
-      <formula>ISBLANK(D83)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G83">
-    <cfRule type="containsText" dxfId="99" priority="197" operator="containsText" text="highlight">
-      <formula>G83="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="198" operator="containsText" text="highlight">
-      <formula>G83="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D84">
-    <cfRule type="containsText" dxfId="97" priority="199" operator="containsText" text="highlight">
-      <formula>ISBLANK(D84)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G84">
-    <cfRule type="containsText" dxfId="96" priority="200" operator="containsText" text="highlight">
-      <formula>G84="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="201" operator="containsText" text="highlight">
-      <formula>G84="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D85">
-    <cfRule type="containsText" dxfId="94" priority="202" operator="containsText" text="highlight">
-      <formula>ISBLANK(D85)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G85">
-    <cfRule type="containsText" dxfId="93" priority="203" operator="containsText" text="highlight">
-      <formula>G85="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="204" operator="containsText" text="highlight">
-      <formula>G85="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D86">
-    <cfRule type="containsText" dxfId="91" priority="205" operator="containsText" text="highlight">
-      <formula>ISBLANK(D86)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G86">
-    <cfRule type="containsText" dxfId="90" priority="206" operator="containsText" text="highlight">
-      <formula>G86="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="207" operator="containsText" text="highlight">
-      <formula>G86="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D87">
-    <cfRule type="containsText" dxfId="88" priority="208" operator="containsText" text="highlight">
-      <formula>ISBLANK(D87)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G87">
-    <cfRule type="containsText" dxfId="87" priority="209" operator="containsText" text="highlight">
-      <formula>G87="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="210" operator="containsText" text="highlight">
-      <formula>G87="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D88">
-    <cfRule type="containsText" dxfId="85" priority="211" operator="containsText" text="highlight">
-      <formula>ISBLANK(D88)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G88">
-    <cfRule type="containsText" dxfId="84" priority="212" operator="containsText" text="highlight">
-      <formula>G88="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="213" operator="containsText" text="highlight">
-      <formula>G88="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D89">
-    <cfRule type="containsText" dxfId="82" priority="214" operator="containsText" text="highlight">
-      <formula>ISBLANK(D89)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G89">
-    <cfRule type="containsText" dxfId="81" priority="215" operator="containsText" text="highlight">
-      <formula>G89="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="216" operator="containsText" text="highlight">
-      <formula>G89="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D91">
-    <cfRule type="containsText" dxfId="79" priority="217" operator="containsText" text="highlight">
-      <formula>ISBLANK(D91)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G91">
-    <cfRule type="containsText" dxfId="78" priority="218" operator="containsText" text="highlight">
+  <conditionalFormatting sqref="G91:G101">
+    <cfRule type="containsText" dxfId="3" priority="218" operator="containsText" text="highlight">
       <formula>G91="Fail"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="219" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="2" priority="219" operator="containsText" text="highlight">
       <formula>G91="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D92">
-    <cfRule type="containsText" dxfId="76" priority="220" operator="containsText" text="highlight">
-      <formula>ISBLANK(D92)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G92">
-    <cfRule type="containsText" dxfId="75" priority="221" operator="containsText" text="highlight">
-      <formula>G92="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="222" operator="containsText" text="highlight">
-      <formula>G92="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D93">
-    <cfRule type="containsText" dxfId="73" priority="223" operator="containsText" text="highlight">
-      <formula>ISBLANK(D93)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G93">
-    <cfRule type="containsText" dxfId="72" priority="224" operator="containsText" text="highlight">
-      <formula>G93="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="225" operator="containsText" text="highlight">
-      <formula>G93="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D94">
-    <cfRule type="containsText" dxfId="70" priority="226" operator="containsText" text="highlight">
-      <formula>ISBLANK(D94)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G94">
-    <cfRule type="containsText" dxfId="69" priority="227" operator="containsText" text="highlight">
-      <formula>G94="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="228" operator="containsText" text="highlight">
-      <formula>G94="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D95">
-    <cfRule type="containsText" dxfId="67" priority="229" operator="containsText" text="highlight">
-      <formula>ISBLANK(D95)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G95">
-    <cfRule type="containsText" dxfId="66" priority="230" operator="containsText" text="highlight">
-      <formula>G95="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="231" operator="containsText" text="highlight">
-      <formula>G95="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D96">
-    <cfRule type="containsText" dxfId="64" priority="232" operator="containsText" text="highlight">
-      <formula>ISBLANK(D96)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G96">
-    <cfRule type="containsText" dxfId="63" priority="233" operator="containsText" text="highlight">
-      <formula>G96="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="234" operator="containsText" text="highlight">
-      <formula>G96="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D97">
-    <cfRule type="containsText" dxfId="61" priority="235" operator="containsText" text="highlight">
-      <formula>ISBLANK(D97)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G97">
-    <cfRule type="containsText" dxfId="60" priority="236" operator="containsText" text="highlight">
-      <formula>G97="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="237" operator="containsText" text="highlight">
-      <formula>G97="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D98">
-    <cfRule type="containsText" dxfId="58" priority="238" operator="containsText" text="highlight">
-      <formula>ISBLANK(D98)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G98">
-    <cfRule type="containsText" dxfId="57" priority="239" operator="containsText" text="highlight">
-      <formula>G98="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="240" operator="containsText" text="highlight">
-      <formula>G98="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D99">
-    <cfRule type="containsText" dxfId="55" priority="241" operator="containsText" text="highlight">
-      <formula>ISBLANK(D99)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G99">
-    <cfRule type="containsText" dxfId="54" priority="242" operator="containsText" text="highlight">
-      <formula>G99="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="243" operator="containsText" text="highlight">
-      <formula>G99="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D100">
-    <cfRule type="containsText" dxfId="52" priority="244" operator="containsText" text="highlight">
-      <formula>ISBLANK(D100)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G100">
-    <cfRule type="containsText" dxfId="51" priority="245" operator="containsText" text="highlight">
-      <formula>G100="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="246" operator="containsText" text="highlight">
-      <formula>G100="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D101">
-    <cfRule type="containsText" dxfId="49" priority="247" operator="containsText" text="highlight">
-      <formula>ISBLANK(D101)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G101">
-    <cfRule type="containsText" dxfId="48" priority="248" operator="containsText" text="highlight">
-      <formula>G101="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="249" operator="containsText" text="highlight">
-      <formula>G101="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D103">
-    <cfRule type="containsText" dxfId="46" priority="250" operator="containsText" text="highlight">
-      <formula>ISBLANK(D103)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G103">
-    <cfRule type="containsText" dxfId="45" priority="251" operator="containsText" text="highlight">
+  <conditionalFormatting sqref="G103:G113">
+    <cfRule type="containsText" dxfId="1" priority="251" operator="containsText" text="highlight">
       <formula>G103="Fail"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="252" operator="containsText" text="highlight">
+    <cfRule type="containsText" dxfId="0" priority="252" operator="containsText" text="highlight">
       <formula>G103="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D104">
-    <cfRule type="containsText" dxfId="43" priority="253" operator="containsText" text="highlight">
-      <formula>ISBLANK(D104)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G104">
-    <cfRule type="containsText" dxfId="42" priority="254" operator="containsText" text="highlight">
-      <formula>G104="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="255" operator="containsText" text="highlight">
-      <formula>G104="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D105">
-    <cfRule type="containsText" dxfId="40" priority="256" operator="containsText" text="highlight">
-      <formula>ISBLANK(D105)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G105">
-    <cfRule type="containsText" dxfId="39" priority="257" operator="containsText" text="highlight">
-      <formula>G105="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="258" operator="containsText" text="highlight">
-      <formula>G105="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D106">
-    <cfRule type="containsText" dxfId="37" priority="259" operator="containsText" text="highlight">
-      <formula>ISBLANK(D106)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G106">
-    <cfRule type="containsText" dxfId="36" priority="260" operator="containsText" text="highlight">
-      <formula>G106="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="261" operator="containsText" text="highlight">
-      <formula>G106="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D107">
-    <cfRule type="containsText" dxfId="34" priority="262" operator="containsText" text="highlight">
-      <formula>ISBLANK(D107)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G107">
-    <cfRule type="containsText" dxfId="33" priority="263" operator="containsText" text="highlight">
-      <formula>G107="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="264" operator="containsText" text="highlight">
-      <formula>G107="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D108">
-    <cfRule type="containsText" dxfId="31" priority="265" operator="containsText" text="highlight">
-      <formula>ISBLANK(D108)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G108">
-    <cfRule type="containsText" dxfId="30" priority="266" operator="containsText" text="highlight">
-      <formula>G108="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="267" operator="containsText" text="highlight">
-      <formula>G108="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D109">
-    <cfRule type="containsText" dxfId="28" priority="268" operator="containsText" text="highlight">
-      <formula>ISBLANK(D109)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G109">
-    <cfRule type="containsText" dxfId="27" priority="269" operator="containsText" text="highlight">
-      <formula>G109="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="270" operator="containsText" text="highlight">
-      <formula>G109="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D110">
-    <cfRule type="containsText" dxfId="25" priority="271" operator="containsText" text="highlight">
-      <formula>ISBLANK(D110)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G110">
-    <cfRule type="containsText" dxfId="24" priority="272" operator="containsText" text="highlight">
-      <formula>G110="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="273" operator="containsText" text="highlight">
-      <formula>G110="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D111">
-    <cfRule type="containsText" dxfId="22" priority="274" operator="containsText" text="highlight">
-      <formula>ISBLANK(D111)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G111">
-    <cfRule type="containsText" dxfId="21" priority="275" operator="containsText" text="highlight">
-      <formula>G111="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="276" operator="containsText" text="highlight">
-      <formula>G111="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D112">
-    <cfRule type="containsText" dxfId="19" priority="277" operator="containsText" text="highlight">
-      <formula>ISBLANK(D112)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G112">
-    <cfRule type="containsText" dxfId="18" priority="278" operator="containsText" text="highlight">
-      <formula>G112="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="279" operator="containsText" text="highlight">
-      <formula>G112="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D113">
-    <cfRule type="containsText" dxfId="16" priority="280" operator="containsText" text="highlight">
-      <formula>ISBLANK(D113)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G113">
-    <cfRule type="containsText" dxfId="15" priority="281" operator="containsText" text="highlight">
-      <formula>G113="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="282" operator="containsText" text="highlight">
-      <formula>G113="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A124">
-    <cfRule type="containsText" dxfId="13" priority="295" operator="containsText" text="highlight">
-      <formula>ISBLANK(A124)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B124">
-    <cfRule type="containsText" dxfId="12" priority="296" operator="containsText" text="highlight">
-      <formula>ISBLANK(B124)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E124">
-    <cfRule type="containsText" dxfId="11" priority="297" operator="containsText" text="highlight">
-      <formula>E124="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="298" operator="containsText" text="highlight">
-      <formula>E124="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C129:C132">
-    <cfRule type="containsText" dxfId="9" priority="303" operator="containsText" text="highlight">
-      <formula>ISBLANK(C129)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="304" operator="containsText" text="highlight">
-      <formula>C129="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="305" operator="containsText" text="highlight">
-      <formula>C129="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B134">
-    <cfRule type="containsText" dxfId="6" priority="309" operator="containsText" text="highlight">
-      <formula>ISBLANK(B134)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F117:F120">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="highlight">
-      <formula>F117="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="highlight">
-      <formula>F117="Pass"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B117:B120">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="highlight">
-      <formula>ISBLANK(B117)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C134">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="highlight">
-      <formula>ISBLANK(C134)</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="highlight">
-      <formula>C134="Fail"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="highlight">
-      <formula>C134="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>